<commit_message>
add oscillator fix board
</commit_message>
<xml_diff>
--- a/Board/bom/cbm_ultipet_v1.2a-bom.xlsx
+++ b/Board/bom/cbm_ultipet_v1.2a-bom.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="867" uniqueCount="727">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="883" uniqueCount="737">
   <si>
     <t xml:space="preserve">Id</t>
   </si>
@@ -258,6 +258,12 @@
     <t xml:space="preserve">1u</t>
   </si>
   <si>
+    <t xml:space="preserve">791-0603B105K6R3CT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0603B105K6R3CT</t>
+  </si>
+  <si>
     <t xml:space="preserve">80-C0603X105J8R</t>
   </si>
   <si>
@@ -579,6 +585,12 @@
     <t xml:space="preserve">pin strip straight 20 pin</t>
   </si>
   <si>
+    <t xml:space="preserve">538-22-28-4204</t>
+  </si>
+  <si>
+    <t xml:space="preserve">22-28-4204</t>
+  </si>
+  <si>
     <t xml:space="preserve">649-1012937892001BLF </t>
   </si>
   <si>
@@ -753,6 +765,9 @@
     <t xml:space="preserve">E2,5-6</t>
   </si>
   <si>
+    <t xml:space="preserve">710-860010772005</t>
+  </si>
+  <si>
     <t xml:space="preserve">710-860020672005 </t>
   </si>
   <si>
@@ -828,7 +843,7 @@
     <t xml:space="preserve">E2-5</t>
   </si>
   <si>
-    <t xml:space="preserve">1u  (note: alternatively mlcc?)</t>
+    <t xml:space="preserve">1u  (note: alternatively mlcc)</t>
   </si>
   <si>
     <t xml:space="preserve">710-860020672005</t>
@@ -1101,6 +1116,12 @@
     <t xml:space="preserve">1k</t>
   </si>
   <si>
+    <t xml:space="preserve">603-MFR-12FRF521K</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MFR-12FRF52-1K</t>
+  </si>
+  <si>
     <t xml:space="preserve">603-MFR-12FTF52-1K</t>
   </si>
   <si>
@@ -1755,18 +1776,18 @@
     <t xml:space="preserve">Socket 44 pin PLCC</t>
   </si>
   <si>
+    <t xml:space="preserve">517-8444-11B1-RK-TP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8444-11B1-RK-TP</t>
+  </si>
+  <si>
     <t xml:space="preserve">737-PLCC-44-AT</t>
   </si>
   <si>
     <t xml:space="preserve">PLCC-44-AT</t>
   </si>
   <si>
-    <t xml:space="preserve">517-8444-11B1-RK-TP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8444-11B1-RK-TP</t>
-  </si>
-  <si>
     <t xml:space="preserve">X4</t>
   </si>
   <si>
@@ -2236,6 +2257,15 @@
   </si>
   <si>
     <t xml:space="preserve">CMS-321437-24SP-X8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Key switches N-Keyboard (for SJGray PCB)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">540-MX1A-C1NW </t>
+  </si>
+  <si>
+    <t xml:space="preserve">MX1A-C1NW </t>
   </si>
 </sst>
 </file>
@@ -2607,10 +2637,14 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L194"/>
+  <dimension ref="A1:L196"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D14" activeCellId="0" sqref="D14:D25"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B164" activePane="bottomRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A164" activeCellId="0" sqref="A164"/>
+      <selection pane="bottomRight" activeCell="B196" activeCellId="0" sqref="B196:I196"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2624,8 +2658,8 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="14.23"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="24.93"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="19.75"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="10" min="10" style="1" width="21.84"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="11" min="11" style="1" width="20.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="21.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="20.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="23.83"/>
   </cols>
   <sheetData>
@@ -2696,7 +2730,7 @@
       <c r="D3" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="E3" s="0"/>
+      <c r="E3" s="1"/>
       <c r="F3" s="1" t="s">
         <v>15</v>
       </c>
@@ -2723,7 +2757,7 @@
       <c r="D4" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="E4" s="0"/>
+      <c r="E4" s="1"/>
       <c r="F4" s="1" t="s">
         <v>21</v>
       </c>
@@ -2750,7 +2784,7 @@
       <c r="D5" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="E5" s="0"/>
+      <c r="E5" s="1"/>
       <c r="F5" s="1" t="s">
         <v>27</v>
       </c>
@@ -2777,7 +2811,7 @@
       <c r="D6" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="E6" s="0"/>
+      <c r="E6" s="1"/>
       <c r="F6" s="1" t="s">
         <v>33</v>
       </c>
@@ -2804,7 +2838,7 @@
       <c r="D7" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="E7" s="0"/>
+      <c r="E7" s="1"/>
       <c r="F7" s="1" t="s">
         <v>39</v>
       </c>
@@ -2855,7 +2889,7 @@
       <c r="D9" s="2" t="n">
         <v>4</v>
       </c>
-      <c r="E9" s="0"/>
+      <c r="E9" s="1"/>
       <c r="F9" s="1" t="s">
         <v>50</v>
       </c>
@@ -2882,7 +2916,7 @@
       <c r="D10" s="2" t="n">
         <v>53</v>
       </c>
-      <c r="E10" s="0"/>
+      <c r="E10" s="1"/>
       <c r="F10" s="1" t="s">
         <v>55</v>
       </c>
@@ -2909,7 +2943,7 @@
       <c r="D11" s="2" t="n">
         <v>9</v>
       </c>
-      <c r="E11" s="0"/>
+      <c r="E11" s="1"/>
       <c r="F11" s="1" t="s">
         <v>61</v>
       </c>
@@ -2936,38 +2970,44 @@
       <c r="D12" s="2" t="n">
         <v>12</v>
       </c>
-      <c r="E12" s="0"/>
+      <c r="E12" s="1"/>
       <c r="F12" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="H12" s="5" t="s">
+      <c r="H12" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="I12" s="5" t="s">
+      <c r="I12" s="1" t="s">
         <v>68</v>
       </c>
+      <c r="J12" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="K12" s="5" t="s">
+        <v>70</v>
+      </c>
       <c r="L12" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="D13" s="2" t="n">
         <v>1</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="H13" s="5" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="I13" s="5" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="L13" s="1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2975,26 +3015,26 @@
         <v>109</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="D14" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="E14" s="0"/>
+      <c r="E14" s="1"/>
       <c r="F14" s="1" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="H14" s="5" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="I14" s="5" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="L14" s="1" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3002,26 +3042,26 @@
         <v>93</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="D15" s="2" t="n">
         <v>3</v>
       </c>
-      <c r="E15" s="0"/>
+      <c r="E15" s="1"/>
       <c r="F15" s="1" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="H15" s="5" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="I15" s="5" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="L15" s="1" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3029,26 +3069,26 @@
         <v>86</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="D16" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="E16" s="0"/>
+      <c r="E16" s="1"/>
       <c r="F16" s="1" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="H16" s="5" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="I16" s="5" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="L16" s="1" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3056,26 +3096,26 @@
         <v>64</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="D17" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="E17" s="0"/>
+      <c r="E17" s="1"/>
       <c r="F17" s="1" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="H17" s="5" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="I17" s="5" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="L17" s="1" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3083,26 +3123,26 @@
         <v>49</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="D18" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="E18" s="0"/>
+      <c r="E18" s="1"/>
       <c r="F18" s="1" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="H18" s="7" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="I18" s="7" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="L18" s="1" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3110,26 +3150,26 @@
         <v>152</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="D19" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="E19" s="0"/>
+      <c r="E19" s="1"/>
       <c r="F19" s="1" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="H19" s="5" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="I19" s="5" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="L19" s="1" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3137,26 +3177,26 @@
         <v>57</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="D20" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="E20" s="0"/>
+      <c r="E20" s="1"/>
       <c r="F20" s="1" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="H20" s="5" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="I20" s="5" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="L20" s="1" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3164,26 +3204,26 @@
         <v>107</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="D21" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="E21" s="0"/>
+      <c r="E21" s="1"/>
       <c r="F21" s="1" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="H21" s="5" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="I21" s="5" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="L21" s="1" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3191,26 +3231,26 @@
         <v>72</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="D22" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="E22" s="0"/>
+      <c r="E22" s="1"/>
       <c r="F22" s="1" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="H22" s="5" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="I22" s="5" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="L22" s="1" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3218,26 +3258,26 @@
         <v>3</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="D23" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="E23" s="0"/>
+      <c r="E23" s="1"/>
       <c r="F23" s="1" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="H23" s="5" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="I23" s="5" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="L23" s="1" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3245,26 +3285,26 @@
         <v>116</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="D24" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="E24" s="0"/>
+      <c r="E24" s="1"/>
       <c r="F24" s="1" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="H24" s="5" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="I24" s="5" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="L24" s="1" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3272,26 +3312,26 @@
         <v>38</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="D25" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="E25" s="0"/>
+      <c r="E25" s="1"/>
       <c r="F25" s="1" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="H25" s="5" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="I25" s="5" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="L25" s="1" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3299,28 +3339,28 @@
         <v>63</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="D26" s="2" t="n">
         <v>2</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="H26" s="7" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="I26" s="7" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="3"/>
       <c r="B27" s="3" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="C27" s="3"/>
       <c r="D27" s="4"/>
@@ -3338,10 +3378,10 @@
         <v>4</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="D28" s="2" t="n">
         <v>0</v>
@@ -3350,7 +3390,7 @@
         <v>1</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3358,10 +3398,10 @@
         <v>143</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="D29" s="2" t="n">
         <v>0</v>
@@ -3370,7 +3410,7 @@
         <v>1</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3378,10 +3418,10 @@
         <v>11</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="D30" s="2" t="n">
         <v>0</v>
@@ -3390,7 +3430,7 @@
         <v>11</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3398,10 +3438,10 @@
         <v>26</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="D31" s="2" t="n">
         <v>0</v>
@@ -3410,7 +3450,7 @@
         <v>9</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3418,10 +3458,10 @@
         <v>35</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="D32" s="2" t="n">
         <v>0</v>
@@ -3430,7 +3470,7 @@
         <v>4</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3438,10 +3478,10 @@
         <v>75</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="D33" s="2" t="n">
         <v>0</v>
@@ -3450,7 +3490,7 @@
         <v>1</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3458,10 +3498,10 @@
         <v>77</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="D34" s="2" t="n">
         <v>0</v>
@@ -3470,7 +3510,7 @@
         <v>2</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3478,10 +3518,10 @@
         <v>112</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="D35" s="2" t="n">
         <v>0</v>
@@ -3490,7 +3530,7 @@
         <v>1</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3498,10 +3538,10 @@
         <v>117</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="D36" s="2" t="n">
         <v>0</v>
@@ -3510,7 +3550,7 @@
         <v>2</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3518,13 +3558,19 @@
         <v>10</v>
       </c>
       <c r="F37" s="5" t="s">
-        <v>173</v>
-      </c>
-      <c r="H37" s="5" t="s">
-        <v>174</v>
-      </c>
-      <c r="I37" s="5" t="s">
         <v>175</v>
+      </c>
+      <c r="H37" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="I37" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="J37" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="K37" s="5" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3537,22 +3583,22 @@
         <v>42</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>176</v>
+        <v>180</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
       <c r="D39" s="2" t="n">
         <v>2</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
       <c r="H39" s="5" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
       <c r="I39" s="5" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3560,22 +3606,22 @@
         <v>128</v>
       </c>
       <c r="B40" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="C40" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="C40" s="1" t="s">
-        <v>177</v>
-      </c>
       <c r="D40" s="2" t="n">
         <v>1</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="H40" s="5" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
       <c r="I40" s="5" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3583,22 +3629,22 @@
         <v>151</v>
       </c>
       <c r="B41" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="D41" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="H41" s="5" t="s">
         <v>183</v>
       </c>
-      <c r="C41" s="1" t="s">
+      <c r="I41" s="5" t="s">
         <v>184</v>
-      </c>
-      <c r="D41" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="F41" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="H41" s="5" t="s">
-        <v>179</v>
-      </c>
-      <c r="I41" s="5" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3606,10 +3652,10 @@
         <v>78</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>186</v>
+        <v>190</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="D43" s="2" t="n">
         <v>0</v>
@@ -3618,7 +3664,7 @@
         <v>1</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>188</v>
+        <v>192</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3626,10 +3672,10 @@
         <v>139</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>189</v>
+        <v>193</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>190</v>
+        <v>194</v>
       </c>
       <c r="D44" s="2" t="n">
         <v>0</v>
@@ -3638,15 +3684,15 @@
         <v>1</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>190</v>
+        <v>194</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B45" s="1" t="s">
-        <v>191</v>
+        <v>195</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>192</v>
+        <v>196</v>
       </c>
       <c r="E45" s="2" t="n">
         <v>1</v>
@@ -3657,10 +3703,10 @@
         <v>1</v>
       </c>
       <c r="H46" s="5" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
       <c r="I46" s="5" t="s">
-        <v>194</v>
+        <v>198</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3668,22 +3714,22 @@
         <v>142</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="D48" s="2" t="n">
         <v>1</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>197</v>
+        <v>201</v>
       </c>
       <c r="H48" s="5" t="s">
-        <v>198</v>
+        <v>202</v>
       </c>
       <c r="I48" s="5" t="s">
-        <v>199</v>
+        <v>203</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3691,22 +3737,22 @@
         <v>95</v>
       </c>
       <c r="B49" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="C49" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="C49" s="1" t="s">
-        <v>196</v>
-      </c>
       <c r="D49" s="2" t="n">
         <v>1</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="H49" s="5" t="s">
-        <v>198</v>
+        <v>202</v>
       </c>
       <c r="I49" s="5" t="s">
-        <v>199</v>
+        <v>203</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3714,19 +3760,19 @@
         <v>85</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>202</v>
+        <v>206</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>203</v>
+        <v>207</v>
       </c>
       <c r="D51" s="2" t="n">
         <v>1</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="I51" s="5" t="s">
-        <v>205</v>
+        <v>209</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3747,22 +3793,22 @@
         <v>130</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>206</v>
+        <v>210</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>207</v>
+        <v>211</v>
       </c>
       <c r="D53" s="2" t="n">
         <v>1</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>208</v>
+        <v>212</v>
       </c>
       <c r="H53" s="7" t="s">
-        <v>209</v>
+        <v>213</v>
       </c>
       <c r="I53" s="7" t="s">
-        <v>210</v>
+        <v>214</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3770,25 +3816,25 @@
         <v>120</v>
       </c>
       <c r="B54" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="C54" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="C54" s="1" t="s">
-        <v>207</v>
-      </c>
       <c r="D54" s="2" t="n">
         <v>1</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="H54" s="5" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="I54" s="5" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
       <c r="J54" s="5" t="s">
-        <v>215</v>
+        <v>219</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3796,25 +3842,25 @@
         <v>8</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>216</v>
+        <v>220</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>207</v>
+        <v>211</v>
       </c>
       <c r="D55" s="2" t="n">
         <v>2</v>
       </c>
       <c r="F55" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="H55" s="5" t="s">
         <v>217</v>
       </c>
-      <c r="H55" s="5" t="s">
-        <v>213</v>
-      </c>
       <c r="I55" s="5" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
       <c r="J55" s="5" t="s">
-        <v>215</v>
+        <v>219</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3822,25 +3868,25 @@
         <v>137</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>218</v>
+        <v>222</v>
       </c>
       <c r="C56" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="D56" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="F56" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="H56" s="7" t="s">
+        <v>225</v>
+      </c>
+      <c r="I56" s="7" t="s">
+        <v>226</v>
+      </c>
+      <c r="J56" s="5" t="s">
         <v>219</v>
-      </c>
-      <c r="D56" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="F56" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="H56" s="7" t="s">
-        <v>221</v>
-      </c>
-      <c r="I56" s="7" t="s">
-        <v>222</v>
-      </c>
-      <c r="J56" s="5" t="s">
-        <v>215</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3848,28 +3894,28 @@
         <v>25</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>223</v>
+        <v>227</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>207</v>
+        <v>211</v>
       </c>
       <c r="D57" s="2" t="n">
         <v>19</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>224</v>
+        <v>228</v>
       </c>
       <c r="H57" s="5" t="s">
-        <v>225</v>
+        <v>229</v>
       </c>
       <c r="I57" s="5" t="s">
-        <v>226</v>
+        <v>230</v>
       </c>
       <c r="J57" s="5" t="s">
-        <v>227</v>
+        <v>231</v>
       </c>
       <c r="K57" s="5" t="s">
-        <v>228</v>
+        <v>232</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3877,28 +3923,28 @@
         <v>33</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>229</v>
+        <v>233</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>219</v>
+        <v>223</v>
       </c>
       <c r="D58" s="2" t="n">
         <v>17</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>224</v>
+        <v>228</v>
       </c>
       <c r="H58" s="5" t="s">
-        <v>225</v>
+        <v>229</v>
       </c>
       <c r="I58" s="5" t="s">
-        <v>226</v>
+        <v>230</v>
       </c>
       <c r="J58" s="5" t="s">
-        <v>227</v>
+        <v>231</v>
       </c>
       <c r="K58" s="5" t="s">
-        <v>228</v>
+        <v>232</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3906,10 +3952,10 @@
         <v>96</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>230</v>
+        <v>234</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>231</v>
+        <v>235</v>
       </c>
       <c r="D59" s="2" t="n">
         <v>4</v>
@@ -3917,29 +3963,35 @@
       <c r="F59" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="H59" s="5" t="s">
-        <v>232</v>
-      </c>
-      <c r="I59" s="8" t="s">
-        <v>233</v>
+      <c r="H59" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="I59" s="1" t="n">
+        <v>860010772005</v>
+      </c>
+      <c r="J59" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="K59" s="8" t="s">
+        <v>238</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B60" s="1" t="s">
-        <v>234</v>
+        <v>239</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>235</v>
+        <v>240</v>
       </c>
       <c r="D60" s="2" t="n">
         <v>2</v>
       </c>
       <c r="E60" s="1"/>
       <c r="F60" s="1" t="s">
-        <v>236</v>
+        <v>241</v>
       </c>
       <c r="H60" s="5" t="s">
-        <v>237</v>
+        <v>242</v>
       </c>
       <c r="I60" s="9" t="n">
         <v>860010372006</v>
@@ -3950,43 +4002,43 @@
         <v>9</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>238</v>
+        <v>243</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>231</v>
+        <v>235</v>
       </c>
       <c r="D61" s="2" t="n">
         <v>4</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>239</v>
+        <v>244</v>
       </c>
       <c r="H61" s="5" t="s">
-        <v>240</v>
+        <v>245</v>
       </c>
       <c r="I61" s="5" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B62" s="1" t="s">
-        <v>242</v>
+        <v>247</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>243</v>
+        <v>248</v>
       </c>
       <c r="D62" s="2" t="n">
         <v>2</v>
       </c>
       <c r="E62" s="1"/>
       <c r="F62" s="1" t="s">
-        <v>244</v>
+        <v>249</v>
       </c>
       <c r="H62" s="1" t="s">
-        <v>245</v>
+        <v>250</v>
       </c>
       <c r="I62" s="1" t="s">
-        <v>246</v>
+        <v>251</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3994,42 +4046,42 @@
         <v>28</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>247</v>
+        <v>252</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>219</v>
+        <v>223</v>
       </c>
       <c r="D63" s="2" t="n">
         <v>4</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>248</v>
+        <v>253</v>
       </c>
       <c r="H63" s="7" t="s">
-        <v>249</v>
+        <v>254</v>
       </c>
       <c r="I63" s="7" t="s">
-        <v>250</v>
+        <v>255</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B64" s="1" t="s">
-        <v>251</v>
+        <v>256</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>243</v>
+        <v>248</v>
       </c>
       <c r="D64" s="2" t="n">
         <v>2</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>252</v>
+        <v>257</v>
       </c>
       <c r="H64" s="5" t="s">
-        <v>253</v>
+        <v>258</v>
       </c>
       <c r="I64" s="5" t="s">
-        <v>254</v>
+        <v>259</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4037,22 +4089,28 @@
         <v>45</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>255</v>
+        <v>260</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>256</v>
+        <v>261</v>
       </c>
       <c r="D65" s="2" t="n">
         <v>6</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>257</v>
+        <v>262</v>
       </c>
       <c r="H65" s="5" t="s">
         <v>258</v>
       </c>
       <c r="I65" s="5" t="s">
-        <v>233</v>
+        <v>259</v>
+      </c>
+      <c r="J65" s="5" t="s">
+        <v>263</v>
+      </c>
+      <c r="K65" s="5" t="s">
+        <v>238</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4060,22 +4118,22 @@
         <v>39</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>259</v>
+        <v>264</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>231</v>
+        <v>235</v>
       </c>
       <c r="D66" s="2" t="n">
         <v>2</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>260</v>
+        <v>265</v>
       </c>
       <c r="H66" s="5" t="s">
-        <v>261</v>
+        <v>266</v>
       </c>
       <c r="I66" s="8" t="s">
-        <v>262</v>
+        <v>267</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4083,22 +4141,22 @@
         <v>134</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>263</v>
+        <v>268</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>264</v>
+        <v>269</v>
       </c>
       <c r="D67" s="2" t="n">
         <v>1</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>244</v>
+        <v>249</v>
       </c>
       <c r="H67" s="7" t="s">
-        <v>265</v>
+        <v>270</v>
       </c>
       <c r="I67" s="7" t="s">
-        <v>266</v>
+        <v>271</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4106,22 +4164,22 @@
         <v>103</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>267</v>
+        <v>272</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>256</v>
+        <v>261</v>
       </c>
       <c r="D68" s="2" t="n">
         <v>4</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>244</v>
+        <v>249</v>
       </c>
       <c r="H68" s="7" t="s">
-        <v>265</v>
+        <v>270</v>
       </c>
       <c r="I68" s="7" t="s">
-        <v>266</v>
+        <v>271</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4129,10 +4187,10 @@
         <v>53</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>268</v>
+        <v>273</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>231</v>
+        <v>235</v>
       </c>
       <c r="D69" s="2" t="n">
         <v>1</v>
@@ -4141,10 +4199,10 @@
         <v>61</v>
       </c>
       <c r="H69" s="5" t="s">
-        <v>269</v>
+        <v>274</v>
       </c>
       <c r="I69" s="5" t="s">
-        <v>270</v>
+        <v>275</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4152,22 +4210,22 @@
         <v>65</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>271</v>
+        <v>276</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>272</v>
+        <v>277</v>
       </c>
       <c r="D70" s="2" t="n">
         <v>3</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>239</v>
+        <v>244</v>
       </c>
       <c r="H70" s="5" t="s">
-        <v>240</v>
+        <v>245</v>
       </c>
       <c r="I70" s="5" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4175,28 +4233,28 @@
         <v>80</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>273</v>
+        <v>278</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>272</v>
+        <v>277</v>
       </c>
       <c r="D71" s="2" t="n">
         <v>4</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>236</v>
+        <v>241</v>
       </c>
       <c r="H71" s="5" t="s">
-        <v>237</v>
+        <v>242</v>
       </c>
       <c r="I71" s="9" t="n">
         <v>860010372006</v>
       </c>
       <c r="J71" s="7" t="s">
-        <v>274</v>
+        <v>279</v>
       </c>
       <c r="K71" s="7" t="s">
-        <v>275</v>
+        <v>280</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4204,22 +4262,22 @@
         <v>131</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>276</v>
+        <v>281</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>272</v>
+        <v>277</v>
       </c>
       <c r="D72" s="2" t="n">
         <v>1</v>
       </c>
       <c r="F72" s="1" t="s">
-        <v>277</v>
+        <v>282</v>
       </c>
       <c r="H72" s="7" t="s">
-        <v>278</v>
+        <v>283</v>
       </c>
       <c r="I72" s="7" t="s">
-        <v>279</v>
+        <v>284</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4240,19 +4298,19 @@
         <v>140</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>280</v>
+        <v>285</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>281</v>
+        <v>286</v>
       </c>
       <c r="D74" s="2" t="n">
         <v>1</v>
       </c>
       <c r="F74" s="1" t="s">
-        <v>282</v>
+        <v>287</v>
       </c>
       <c r="H74" s="7" t="s">
-        <v>283</v>
+        <v>288</v>
       </c>
       <c r="I74" s="7" t="n">
         <v>744115</v>
@@ -4263,22 +4321,22 @@
         <v>147</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>284</v>
+        <v>289</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>285</v>
+        <v>290</v>
       </c>
       <c r="D75" s="2" t="n">
         <v>1</v>
       </c>
       <c r="F75" s="1" t="s">
-        <v>286</v>
+        <v>291</v>
       </c>
       <c r="H75" s="7" t="s">
-        <v>287</v>
+        <v>292</v>
       </c>
       <c r="I75" s="7" t="s">
-        <v>288</v>
+        <v>293</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4299,28 +4357,28 @@
         <v>6</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>289</v>
+        <v>294</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>290</v>
+        <v>295</v>
       </c>
       <c r="D77" s="2" t="n">
         <v>2</v>
       </c>
       <c r="F77" s="1" t="s">
-        <v>291</v>
+        <v>296</v>
       </c>
       <c r="H77" s="5" t="s">
-        <v>292</v>
+        <v>297</v>
       </c>
       <c r="I77" s="5" t="s">
-        <v>293</v>
+        <v>298</v>
       </c>
       <c r="J77" s="7" t="s">
-        <v>294</v>
+        <v>299</v>
       </c>
       <c r="K77" s="7" t="s">
-        <v>295</v>
+        <v>300</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4328,22 +4386,22 @@
         <v>74</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>296</v>
+        <v>301</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>290</v>
+        <v>295</v>
       </c>
       <c r="D78" s="2" t="n">
         <v>1</v>
       </c>
       <c r="F78" s="1" t="s">
-        <v>297</v>
+        <v>302</v>
       </c>
       <c r="H78" s="5" t="s">
-        <v>298</v>
+        <v>303</v>
       </c>
       <c r="I78" s="5" t="s">
-        <v>299</v>
+        <v>304</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4351,22 +4409,22 @@
         <v>125</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>300</v>
+        <v>305</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>290</v>
+        <v>295</v>
       </c>
       <c r="D79" s="2" t="n">
         <v>1</v>
       </c>
       <c r="F79" s="1" t="s">
-        <v>301</v>
+        <v>306</v>
       </c>
       <c r="H79" s="7" t="s">
-        <v>302</v>
+        <v>307</v>
       </c>
       <c r="I79" s="7" t="s">
-        <v>303</v>
+        <v>308</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4374,22 +4432,22 @@
         <v>135</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>304</v>
+        <v>309</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>305</v>
+        <v>310</v>
       </c>
       <c r="D80" s="2" t="n">
         <v>1</v>
       </c>
       <c r="F80" s="1" t="s">
-        <v>306</v>
+        <v>311</v>
       </c>
       <c r="H80" s="5" t="s">
-        <v>307</v>
+        <v>312</v>
       </c>
       <c r="I80" s="5" t="s">
-        <v>308</v>
+        <v>313</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4410,22 +4468,22 @@
         <v>92</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>309</v>
+        <v>314</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>310</v>
+        <v>315</v>
       </c>
       <c r="D82" s="2" t="n">
         <v>1</v>
       </c>
       <c r="F82" s="1" t="s">
-        <v>311</v>
+        <v>316</v>
       </c>
       <c r="H82" s="7" t="s">
-        <v>312</v>
+        <v>317</v>
       </c>
       <c r="I82" s="7" t="s">
-        <v>313</v>
+        <v>318</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4433,10 +4491,10 @@
         <v>12</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>314</v>
+        <v>319</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>315</v>
+        <v>320</v>
       </c>
       <c r="D83" s="2" t="n">
         <v>1</v>
@@ -4445,10 +4503,10 @@
         <v>10</v>
       </c>
       <c r="H83" s="5" t="s">
-        <v>316</v>
+        <v>321</v>
       </c>
       <c r="I83" s="5" t="s">
-        <v>317</v>
+        <v>322</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4456,10 +4514,10 @@
         <v>24</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>318</v>
+        <v>323</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>310</v>
+        <v>315</v>
       </c>
       <c r="D84" s="2" t="n">
         <v>3</v>
@@ -4468,10 +4526,10 @@
         <v>33</v>
       </c>
       <c r="H84" s="5" t="s">
-        <v>319</v>
+        <v>324</v>
       </c>
       <c r="I84" s="5" t="s">
-        <v>320</v>
+        <v>325</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4479,10 +4537,10 @@
         <v>44</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>321</v>
+        <v>326</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>322</v>
+        <v>327</v>
       </c>
       <c r="D85" s="2" t="n">
         <v>2</v>
@@ -4491,10 +4549,10 @@
         <v>68</v>
       </c>
       <c r="H85" s="5" t="s">
-        <v>323</v>
+        <v>328</v>
       </c>
       <c r="I85" s="5" t="s">
-        <v>324</v>
+        <v>329</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4502,10 +4560,10 @@
         <v>84</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>325</v>
+        <v>330</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>322</v>
+        <v>327</v>
       </c>
       <c r="D86" s="2" t="n">
         <v>3</v>
@@ -4514,10 +4572,10 @@
         <v>100</v>
       </c>
       <c r="H86" s="5" t="s">
-        <v>326</v>
+        <v>331</v>
       </c>
       <c r="I86" s="5" t="s">
-        <v>327</v>
+        <v>332</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4525,10 +4583,10 @@
         <v>146</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>328</v>
+        <v>333</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>310</v>
+        <v>315</v>
       </c>
       <c r="D87" s="2" t="n">
         <v>1</v>
@@ -4537,10 +4595,10 @@
         <v>180</v>
       </c>
       <c r="H87" s="5" t="s">
-        <v>329</v>
+        <v>334</v>
       </c>
       <c r="I87" s="5" t="s">
-        <v>330</v>
+        <v>335</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4548,10 +4606,10 @@
         <v>56</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>331</v>
+        <v>336</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>332</v>
+        <v>337</v>
       </c>
       <c r="D88" s="2" t="n">
         <v>1</v>
@@ -4560,10 +4618,10 @@
         <v>330</v>
       </c>
       <c r="H88" s="5" t="s">
-        <v>333</v>
+        <v>338</v>
       </c>
       <c r="I88" s="5" t="s">
-        <v>334</v>
+        <v>339</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4571,10 +4629,10 @@
         <v>55</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>335</v>
+        <v>340</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>332</v>
+        <v>337</v>
       </c>
       <c r="D89" s="2" t="n">
         <v>2</v>
@@ -4583,16 +4641,16 @@
         <v>390</v>
       </c>
       <c r="H89" s="5" t="s">
-        <v>336</v>
+        <v>341</v>
       </c>
       <c r="I89" s="5" t="s">
-        <v>337</v>
+        <v>342</v>
       </c>
       <c r="J89" s="5" t="s">
-        <v>338</v>
+        <v>343</v>
       </c>
       <c r="K89" s="5" t="s">
-        <v>339</v>
+        <v>344</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4600,10 +4658,10 @@
         <v>32</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>340</v>
+        <v>345</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>310</v>
+        <v>315</v>
       </c>
       <c r="D90" s="2" t="n">
         <v>6</v>
@@ -4612,10 +4670,10 @@
         <v>470</v>
       </c>
       <c r="H90" s="5" t="s">
-        <v>341</v>
+        <v>346</v>
       </c>
       <c r="I90" s="5" t="s">
-        <v>342</v>
+        <v>347</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4623,10 +4681,10 @@
         <v>40</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>343</v>
+        <v>348</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>344</v>
+        <v>349</v>
       </c>
       <c r="D91" s="2" t="n">
         <v>1</v>
@@ -4635,10 +4693,10 @@
         <v>470</v>
       </c>
       <c r="H91" s="5" t="s">
-        <v>341</v>
+        <v>346</v>
       </c>
       <c r="I91" s="5" t="s">
-        <v>342</v>
+        <v>347</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4646,10 +4704,10 @@
         <v>113</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>345</v>
+        <v>350</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>322</v>
+        <v>327</v>
       </c>
       <c r="D92" s="2" t="n">
         <v>3</v>
@@ -4658,10 +4716,10 @@
         <v>470</v>
       </c>
       <c r="H92" s="5" t="s">
-        <v>341</v>
+        <v>346</v>
       </c>
       <c r="I92" s="5" t="s">
-        <v>342</v>
+        <v>347</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4669,22 +4727,28 @@
         <v>153</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>346</v>
+        <v>351</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>315</v>
+        <v>320</v>
       </c>
       <c r="D93" s="2" t="n">
         <v>1</v>
       </c>
       <c r="F93" s="1" t="s">
-        <v>347</v>
-      </c>
-      <c r="H93" s="5" t="s">
-        <v>348</v>
-      </c>
-      <c r="I93" s="5" t="s">
-        <v>349</v>
+        <v>352</v>
+      </c>
+      <c r="H93" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="I93" s="1" t="s">
+        <v>354</v>
+      </c>
+      <c r="J93" s="5" t="s">
+        <v>355</v>
+      </c>
+      <c r="K93" s="5" t="s">
+        <v>356</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4692,22 +4756,28 @@
         <v>110</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>350</v>
+        <v>357</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>332</v>
+        <v>337</v>
       </c>
       <c r="D94" s="2" t="n">
         <v>1</v>
       </c>
       <c r="F94" s="1" t="s">
-        <v>347</v>
-      </c>
-      <c r="H94" s="5" t="s">
-        <v>348</v>
-      </c>
-      <c r="I94" s="5" t="s">
-        <v>349</v>
+        <v>352</v>
+      </c>
+      <c r="H94" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="I94" s="1" t="s">
+        <v>354</v>
+      </c>
+      <c r="J94" s="5" t="s">
+        <v>355</v>
+      </c>
+      <c r="K94" s="5" t="s">
+        <v>356</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4715,22 +4785,28 @@
         <v>111</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>351</v>
+        <v>358</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>322</v>
+        <v>327</v>
       </c>
       <c r="D95" s="2" t="n">
         <v>4</v>
       </c>
       <c r="F95" s="1" t="s">
-        <v>347</v>
-      </c>
-      <c r="H95" s="5" t="s">
-        <v>348</v>
-      </c>
-      <c r="I95" s="5" t="s">
-        <v>349</v>
+        <v>352</v>
+      </c>
+      <c r="H95" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="I95" s="1" t="s">
+        <v>354</v>
+      </c>
+      <c r="J95" s="5" t="s">
+        <v>355</v>
+      </c>
+      <c r="K95" s="5" t="s">
+        <v>356</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4738,22 +4814,22 @@
         <v>100</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>352</v>
+        <v>359</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>310</v>
+        <v>315</v>
       </c>
       <c r="D96" s="2" t="n">
         <v>1</v>
       </c>
       <c r="F96" s="1" t="s">
-        <v>353</v>
+        <v>360</v>
       </c>
       <c r="H96" s="7" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
       <c r="I96" s="7" t="s">
-        <v>355</v>
+        <v>362</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4761,22 +4837,22 @@
         <v>104</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>356</v>
+        <v>363</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>322</v>
+        <v>327</v>
       </c>
       <c r="D97" s="2" t="n">
         <v>1</v>
       </c>
       <c r="F97" s="1" t="s">
-        <v>357</v>
+        <v>364</v>
       </c>
       <c r="H97" s="5" t="s">
-        <v>358</v>
+        <v>365</v>
       </c>
       <c r="I97" s="5" t="s">
-        <v>359</v>
+        <v>366</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4784,22 +4860,22 @@
         <v>157</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>360</v>
+        <v>367</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>332</v>
+        <v>337</v>
       </c>
       <c r="D98" s="2" t="n">
         <v>1</v>
       </c>
       <c r="F98" s="1" t="s">
-        <v>357</v>
+        <v>364</v>
       </c>
       <c r="H98" s="5" t="s">
-        <v>358</v>
+        <v>365</v>
       </c>
       <c r="I98" s="5" t="s">
-        <v>359</v>
+        <v>366</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4807,22 +4883,22 @@
         <v>41</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>361</v>
+        <v>368</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>322</v>
+        <v>327</v>
       </c>
       <c r="D99" s="2" t="n">
         <v>2</v>
       </c>
       <c r="F99" s="1" t="s">
-        <v>362</v>
+        <v>369</v>
       </c>
       <c r="H99" s="5" t="s">
-        <v>363</v>
+        <v>370</v>
       </c>
       <c r="I99" s="5" t="s">
-        <v>364</v>
+        <v>371</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4830,28 +4906,28 @@
         <v>62</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>365</v>
+        <v>372</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>332</v>
+        <v>337</v>
       </c>
       <c r="D100" s="2" t="n">
         <v>3</v>
       </c>
       <c r="F100" s="1" t="s">
-        <v>366</v>
+        <v>373</v>
       </c>
       <c r="H100" s="5" t="s">
-        <v>367</v>
+        <v>374</v>
       </c>
       <c r="I100" s="5" t="s">
-        <v>368</v>
+        <v>375</v>
       </c>
       <c r="J100" s="5" t="s">
-        <v>369</v>
+        <v>376</v>
       </c>
       <c r="K100" s="5" t="s">
-        <v>370</v>
+        <v>377</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4859,22 +4935,22 @@
         <v>17</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>371</v>
+        <v>378</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>310</v>
+        <v>315</v>
       </c>
       <c r="D101" s="2" t="n">
         <v>1</v>
       </c>
       <c r="F101" s="1" t="s">
-        <v>372</v>
+        <v>379</v>
       </c>
       <c r="H101" s="5" t="s">
-        <v>373</v>
+        <v>380</v>
       </c>
       <c r="I101" s="5" t="s">
-        <v>374</v>
+        <v>381</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4882,22 +4958,22 @@
         <v>105</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>375</v>
+        <v>382</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>376</v>
+        <v>383</v>
       </c>
       <c r="D102" s="2" t="n">
         <v>2</v>
       </c>
       <c r="F102" s="1" t="s">
-        <v>377</v>
+        <v>384</v>
       </c>
       <c r="H102" s="5" t="s">
-        <v>378</v>
+        <v>385</v>
       </c>
       <c r="I102" s="5" t="s">
-        <v>379</v>
+        <v>386</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4905,22 +4981,22 @@
         <v>15</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>380</v>
+        <v>387</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>332</v>
+        <v>337</v>
       </c>
       <c r="D103" s="2" t="n">
         <v>5</v>
       </c>
       <c r="F103" s="1" t="s">
-        <v>377</v>
+        <v>384</v>
       </c>
       <c r="H103" s="5" t="s">
-        <v>378</v>
+        <v>385</v>
       </c>
       <c r="I103" s="5" t="s">
-        <v>379</v>
+        <v>386</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4928,22 +5004,22 @@
         <v>71</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>381</v>
+        <v>388</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>344</v>
+        <v>349</v>
       </c>
       <c r="D104" s="2" t="n">
         <v>1</v>
       </c>
       <c r="F104" s="1" t="s">
-        <v>377</v>
+        <v>384</v>
       </c>
       <c r="H104" s="5" t="s">
-        <v>378</v>
+        <v>385</v>
       </c>
       <c r="I104" s="5" t="s">
-        <v>379</v>
+        <v>386</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4951,22 +5027,22 @@
         <v>52</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>382</v>
+        <v>389</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>315</v>
+        <v>320</v>
       </c>
       <c r="D105" s="2" t="n">
         <v>2</v>
       </c>
       <c r="F105" s="1" t="s">
-        <v>377</v>
+        <v>384</v>
       </c>
       <c r="H105" s="5" t="s">
-        <v>378</v>
+        <v>385</v>
       </c>
       <c r="I105" s="5" t="s">
-        <v>379</v>
+        <v>386</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4974,22 +5050,22 @@
         <v>129</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>383</v>
+        <v>390</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>344</v>
+        <v>349</v>
       </c>
       <c r="D106" s="2" t="n">
         <v>1</v>
       </c>
       <c r="F106" s="1" t="s">
-        <v>384</v>
+        <v>391</v>
       </c>
       <c r="H106" s="7" t="s">
-        <v>385</v>
+        <v>392</v>
       </c>
       <c r="I106" s="7" t="s">
-        <v>386</v>
+        <v>393</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4997,25 +5073,25 @@
         <v>51</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>387</v>
+        <v>394</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>310</v>
+        <v>315</v>
       </c>
       <c r="D107" s="2" t="n">
         <v>2</v>
       </c>
       <c r="F107" s="1" t="s">
-        <v>388</v>
+        <v>395</v>
       </c>
       <c r="H107" s="5" t="s">
-        <v>389</v>
+        <v>396</v>
       </c>
       <c r="I107" s="7" t="s">
-        <v>390</v>
+        <v>397</v>
       </c>
       <c r="J107" s="6" t="s">
-        <v>391</v>
+        <v>398</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5023,22 +5099,22 @@
         <v>108</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>392</v>
+        <v>399</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>332</v>
+        <v>337</v>
       </c>
       <c r="D108" s="2" t="n">
         <v>1</v>
       </c>
       <c r="F108" s="1" t="s">
-        <v>393</v>
+        <v>400</v>
       </c>
       <c r="H108" s="7" t="s">
-        <v>394</v>
+        <v>401</v>
       </c>
       <c r="I108" s="7" t="s">
-        <v>395</v>
+        <v>402</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5046,22 +5122,22 @@
         <v>13</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>396</v>
+        <v>403</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>310</v>
+        <v>315</v>
       </c>
       <c r="D109" s="2" t="n">
         <v>8</v>
       </c>
       <c r="F109" s="1" t="s">
-        <v>393</v>
+        <v>400</v>
       </c>
       <c r="H109" s="7" t="s">
-        <v>394</v>
+        <v>401</v>
       </c>
       <c r="I109" s="7" t="s">
-        <v>395</v>
+        <v>402</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5069,22 +5145,22 @@
         <v>36</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>397</v>
+        <v>404</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>344</v>
+        <v>349</v>
       </c>
       <c r="D110" s="2" t="n">
         <v>3</v>
       </c>
       <c r="F110" s="1" t="s">
-        <v>393</v>
+        <v>400</v>
       </c>
       <c r="H110" s="7" t="s">
-        <v>394</v>
+        <v>401</v>
       </c>
       <c r="I110" s="7" t="s">
-        <v>395</v>
+        <v>402</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5092,28 +5168,28 @@
         <v>10</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>398</v>
+        <v>405</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>310</v>
+        <v>315</v>
       </c>
       <c r="D111" s="2" t="n">
         <v>4</v>
       </c>
       <c r="F111" s="1" t="s">
-        <v>399</v>
+        <v>406</v>
       </c>
       <c r="H111" s="5" t="s">
-        <v>400</v>
+        <v>407</v>
       </c>
       <c r="I111" s="5" t="s">
-        <v>401</v>
+        <v>408</v>
       </c>
       <c r="J111" s="7" t="s">
-        <v>402</v>
+        <v>409</v>
       </c>
       <c r="K111" s="7" t="s">
-        <v>403</v>
+        <v>410</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5121,22 +5197,22 @@
         <v>19</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>404</v>
+        <v>411</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>405</v>
+        <v>412</v>
       </c>
       <c r="D112" s="2" t="n">
         <v>1</v>
       </c>
       <c r="F112" s="1" t="s">
-        <v>406</v>
+        <v>413</v>
       </c>
       <c r="H112" s="1" t="s">
-        <v>407</v>
+        <v>414</v>
       </c>
       <c r="I112" s="10" t="s">
-        <v>408</v>
+        <v>415</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5144,22 +5220,22 @@
         <v>54</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>409</v>
+        <v>416</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>410</v>
+        <v>417</v>
       </c>
       <c r="D113" s="2" t="n">
         <v>2</v>
       </c>
       <c r="F113" s="1" t="s">
-        <v>377</v>
+        <v>384</v>
       </c>
       <c r="H113" s="5" t="s">
-        <v>411</v>
+        <v>418</v>
       </c>
       <c r="I113" s="5" t="s">
-        <v>412</v>
+        <v>419</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5167,22 +5243,22 @@
         <v>22</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>413</v>
+        <v>420</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>410</v>
+        <v>417</v>
       </c>
       <c r="D114" s="2" t="n">
         <v>2</v>
       </c>
       <c r="F114" s="1" t="s">
-        <v>414</v>
+        <v>421</v>
       </c>
       <c r="H114" s="5" t="s">
-        <v>415</v>
+        <v>422</v>
       </c>
       <c r="I114" s="5" t="s">
-        <v>416</v>
+        <v>423</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5190,28 +5266,28 @@
         <v>46</v>
       </c>
       <c r="B115" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="C115" s="1" t="s">
         <v>417</v>
-      </c>
-      <c r="C115" s="1" t="s">
-        <v>410</v>
       </c>
       <c r="D115" s="2" t="n">
         <v>2</v>
       </c>
       <c r="F115" s="1" t="s">
-        <v>418</v>
+        <v>425</v>
       </c>
       <c r="H115" s="1" t="s">
-        <v>419</v>
+        <v>426</v>
       </c>
       <c r="I115" s="1" t="s">
-        <v>420</v>
+        <v>427</v>
       </c>
       <c r="J115" s="5" t="s">
-        <v>421</v>
+        <v>428</v>
       </c>
       <c r="K115" s="5" t="s">
-        <v>422</v>
+        <v>429</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5219,28 +5295,28 @@
         <v>88</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>423</v>
+        <v>430</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>424</v>
+        <v>431</v>
       </c>
       <c r="D116" s="2" t="n">
         <v>1</v>
       </c>
       <c r="F116" s="1" t="s">
-        <v>366</v>
+        <v>373</v>
       </c>
       <c r="H116" s="1" t="s">
-        <v>425</v>
+        <v>432</v>
       </c>
       <c r="I116" s="1" t="s">
-        <v>426</v>
+        <v>433</v>
       </c>
       <c r="J116" s="5" t="s">
-        <v>427</v>
+        <v>434</v>
       </c>
       <c r="K116" s="5" t="s">
-        <v>428</v>
+        <v>435</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5248,22 +5324,22 @@
         <v>29</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>429</v>
+        <v>436</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>424</v>
+        <v>431</v>
       </c>
       <c r="D117" s="2" t="n">
         <v>1</v>
       </c>
       <c r="F117" s="1" t="s">
-        <v>377</v>
+        <v>384</v>
       </c>
       <c r="H117" s="5" t="s">
-        <v>430</v>
+        <v>437</v>
       </c>
       <c r="I117" s="5" t="s">
-        <v>431</v>
+        <v>438</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5284,43 +5360,43 @@
         <v>1</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>432</v>
+        <v>439</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>433</v>
+        <v>440</v>
       </c>
       <c r="D119" s="2" t="n">
         <v>1</v>
       </c>
       <c r="F119" s="1" t="s">
-        <v>434</v>
+        <v>441</v>
       </c>
       <c r="H119" s="5" t="s">
-        <v>435</v>
+        <v>442</v>
       </c>
       <c r="I119" s="5" t="s">
-        <v>436</v>
+        <v>443</v>
       </c>
       <c r="J119" s="5"/>
     </row>
     <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B120" s="1" t="s">
-        <v>437</v>
+        <v>444</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>438</v>
+        <v>445</v>
       </c>
       <c r="D120" s="2" t="n">
         <v>1</v>
       </c>
       <c r="F120" s="1" t="s">
-        <v>439</v>
+        <v>446</v>
       </c>
       <c r="H120" s="5" t="s">
-        <v>440</v>
+        <v>447</v>
       </c>
       <c r="I120" s="5" t="s">
-        <v>441</v>
+        <v>448</v>
       </c>
       <c r="J120" s="5"/>
     </row>
@@ -5329,22 +5405,22 @@
         <v>18</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>442</v>
+        <v>449</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>433</v>
+        <v>440</v>
       </c>
       <c r="D121" s="2" t="n">
         <v>1</v>
       </c>
       <c r="F121" s="1" t="s">
-        <v>443</v>
+        <v>450</v>
       </c>
       <c r="H121" s="5" t="s">
-        <v>444</v>
+        <v>451</v>
       </c>
       <c r="I121" s="5" t="s">
-        <v>445</v>
+        <v>452</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5352,22 +5428,22 @@
         <v>14</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>446</v>
+        <v>453</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>447</v>
+        <v>454</v>
       </c>
       <c r="D122" s="2" t="n">
         <v>2</v>
       </c>
       <c r="F122" s="1" t="s">
-        <v>448</v>
+        <v>455</v>
       </c>
       <c r="H122" s="5" t="s">
-        <v>449</v>
+        <v>456</v>
       </c>
       <c r="I122" s="5" t="s">
-        <v>450</v>
+        <v>457</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5375,22 +5451,22 @@
         <v>7</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>451</v>
+        <v>458</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>452</v>
+        <v>459</v>
       </c>
       <c r="D123" s="2" t="n">
         <v>1</v>
       </c>
       <c r="F123" s="1" t="s">
-        <v>453</v>
+        <v>460</v>
       </c>
       <c r="H123" s="7" t="s">
-        <v>454</v>
+        <v>461</v>
       </c>
       <c r="I123" s="7" t="s">
-        <v>455</v>
+        <v>462</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5398,22 +5474,22 @@
         <v>30</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>456</v>
+        <v>463</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>457</v>
+        <v>464</v>
       </c>
       <c r="D124" s="2" t="n">
         <v>2</v>
       </c>
       <c r="F124" s="1" t="s">
-        <v>458</v>
+        <v>465</v>
       </c>
       <c r="H124" s="7" t="s">
-        <v>459</v>
+        <v>466</v>
       </c>
       <c r="I124" s="7" t="s">
-        <v>460</v>
+        <v>467</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5421,22 +5497,22 @@
         <v>43</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>461</v>
+        <v>468</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>452</v>
+        <v>459</v>
       </c>
       <c r="D125" s="2" t="n">
         <v>2</v>
       </c>
       <c r="F125" s="1" t="s">
-        <v>462</v>
+        <v>469</v>
       </c>
       <c r="H125" s="5" t="s">
-        <v>463</v>
+        <v>470</v>
       </c>
       <c r="I125" s="5" t="s">
-        <v>464</v>
+        <v>471</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5444,16 +5520,16 @@
         <v>47</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>465</v>
+        <v>472</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>466</v>
+        <v>473</v>
       </c>
       <c r="D126" s="2" t="n">
         <v>2</v>
       </c>
       <c r="F126" s="1" t="s">
-        <v>467</v>
+        <v>474</v>
       </c>
       <c r="H126" s="11"/>
       <c r="I126" s="11"/>
@@ -5463,22 +5539,22 @@
         <v>66</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>468</v>
+        <v>475</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>469</v>
+        <v>476</v>
       </c>
       <c r="D127" s="2" t="n">
         <v>2</v>
       </c>
       <c r="F127" s="1" t="s">
-        <v>470</v>
+        <v>477</v>
       </c>
       <c r="H127" s="5" t="s">
-        <v>471</v>
+        <v>478</v>
       </c>
       <c r="I127" s="5" t="s">
-        <v>472</v>
+        <v>479</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5486,22 +5562,22 @@
         <v>76</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>473</v>
+        <v>480</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>433</v>
+        <v>440</v>
       </c>
       <c r="D128" s="2" t="n">
         <v>1</v>
       </c>
       <c r="F128" s="1" t="s">
-        <v>474</v>
+        <v>481</v>
       </c>
       <c r="H128" s="5" t="s">
-        <v>475</v>
+        <v>482</v>
       </c>
       <c r="I128" s="5" t="s">
-        <v>476</v>
+        <v>483</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5509,22 +5585,22 @@
         <v>73</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>477</v>
+        <v>484</v>
       </c>
       <c r="C129" s="1" t="s">
-        <v>478</v>
+        <v>485</v>
       </c>
       <c r="D129" s="2" t="n">
         <v>2</v>
       </c>
       <c r="F129" s="1" t="s">
-        <v>479</v>
+        <v>486</v>
       </c>
       <c r="H129" s="5" t="s">
-        <v>480</v>
+        <v>487</v>
       </c>
       <c r="I129" s="8" t="s">
-        <v>481</v>
+        <v>488</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5532,22 +5608,22 @@
         <v>90</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>482</v>
+        <v>489</v>
       </c>
       <c r="C130" s="1" t="s">
-        <v>447</v>
+        <v>454</v>
       </c>
       <c r="D130" s="2" t="n">
         <v>2</v>
       </c>
       <c r="F130" s="1" t="s">
-        <v>483</v>
+        <v>490</v>
       </c>
       <c r="H130" s="5" t="s">
-        <v>484</v>
+        <v>491</v>
       </c>
       <c r="I130" s="8" t="s">
-        <v>485</v>
+        <v>492</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5555,22 +5631,22 @@
         <v>97</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>486</v>
+        <v>493</v>
       </c>
       <c r="C131" s="1" t="s">
-        <v>433</v>
+        <v>440</v>
       </c>
       <c r="D131" s="2" t="n">
         <v>1</v>
       </c>
       <c r="F131" s="1" t="s">
-        <v>487</v>
+        <v>494</v>
       </c>
       <c r="H131" s="7" t="s">
-        <v>488</v>
+        <v>495</v>
       </c>
       <c r="I131" s="7" t="s">
-        <v>489</v>
+        <v>496</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5578,22 +5654,22 @@
         <v>101</v>
       </c>
       <c r="B132" s="1" t="s">
-        <v>490</v>
+        <v>497</v>
       </c>
       <c r="C132" s="1" t="s">
-        <v>478</v>
+        <v>485</v>
       </c>
       <c r="D132" s="2" t="n">
         <v>4</v>
       </c>
       <c r="F132" s="1" t="s">
-        <v>491</v>
+        <v>498</v>
       </c>
       <c r="H132" s="5" t="s">
-        <v>492</v>
+        <v>499</v>
       </c>
       <c r="I132" s="8" t="s">
-        <v>493</v>
+        <v>500</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5601,28 +5677,28 @@
         <v>106</v>
       </c>
       <c r="B133" s="1" t="s">
-        <v>494</v>
+        <v>501</v>
       </c>
       <c r="C133" s="1" t="s">
-        <v>433</v>
+        <v>440</v>
       </c>
       <c r="D133" s="2" t="n">
         <v>1</v>
       </c>
       <c r="F133" s="1" t="s">
-        <v>495</v>
+        <v>502</v>
       </c>
       <c r="H133" s="5" t="s">
-        <v>496</v>
+        <v>503</v>
       </c>
       <c r="I133" s="5" t="s">
-        <v>497</v>
+        <v>504</v>
       </c>
       <c r="J133" s="5" t="s">
-        <v>498</v>
+        <v>505</v>
       </c>
       <c r="K133" s="8" t="s">
-        <v>499</v>
+        <v>506</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5630,22 +5706,22 @@
         <v>114</v>
       </c>
       <c r="B134" s="1" t="s">
-        <v>500</v>
+        <v>507</v>
       </c>
       <c r="C134" s="1" t="s">
-        <v>501</v>
+        <v>508</v>
       </c>
       <c r="D134" s="2" t="n">
         <v>1</v>
       </c>
       <c r="F134" s="1" t="s">
-        <v>502</v>
+        <v>509</v>
       </c>
       <c r="H134" s="5" t="s">
-        <v>503</v>
+        <v>510</v>
       </c>
       <c r="I134" s="5" t="s">
-        <v>504</v>
+        <v>511</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5653,22 +5729,22 @@
         <v>118</v>
       </c>
       <c r="B135" s="1" t="s">
-        <v>505</v>
+        <v>512</v>
       </c>
       <c r="C135" s="1" t="s">
-        <v>433</v>
+        <v>440</v>
       </c>
       <c r="D135" s="2" t="n">
         <v>1</v>
       </c>
       <c r="F135" s="1" t="s">
-        <v>506</v>
+        <v>513</v>
       </c>
       <c r="H135" s="5" t="s">
-        <v>507</v>
+        <v>514</v>
       </c>
       <c r="I135" s="5" t="s">
-        <v>508</v>
+        <v>515</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5676,22 +5752,22 @@
         <v>119</v>
       </c>
       <c r="B136" s="1" t="s">
-        <v>509</v>
+        <v>516</v>
       </c>
       <c r="C136" s="1" t="s">
-        <v>433</v>
+        <v>440</v>
       </c>
       <c r="D136" s="2" t="n">
         <v>1</v>
       </c>
       <c r="F136" s="1" t="s">
-        <v>510</v>
+        <v>517</v>
       </c>
       <c r="H136" s="5" t="s">
-        <v>507</v>
+        <v>514</v>
       </c>
       <c r="I136" s="5" t="s">
-        <v>508</v>
+        <v>515</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5699,22 +5775,22 @@
         <v>123</v>
       </c>
       <c r="B137" s="1" t="s">
-        <v>437</v>
+        <v>444</v>
       </c>
       <c r="C137" s="1" t="s">
-        <v>511</v>
+        <v>518</v>
       </c>
       <c r="D137" s="2" t="n">
         <v>1</v>
       </c>
       <c r="F137" s="1" t="s">
-        <v>512</v>
+        <v>519</v>
       </c>
       <c r="H137" s="5" t="s">
-        <v>513</v>
+        <v>520</v>
       </c>
       <c r="I137" s="5" t="s">
-        <v>514</v>
+        <v>521</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5722,22 +5798,22 @@
         <v>124</v>
       </c>
       <c r="B138" s="1" t="s">
-        <v>515</v>
+        <v>522</v>
       </c>
       <c r="C138" s="1" t="s">
-        <v>469</v>
+        <v>476</v>
       </c>
       <c r="D138" s="2" t="n">
         <v>1</v>
       </c>
       <c r="F138" s="1" t="s">
-        <v>516</v>
+        <v>523</v>
       </c>
       <c r="H138" s="5" t="s">
-        <v>517</v>
+        <v>524</v>
       </c>
       <c r="I138" s="5" t="s">
-        <v>518</v>
+        <v>525</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5745,22 +5821,22 @@
         <v>127</v>
       </c>
       <c r="B139" s="1" t="s">
-        <v>519</v>
+        <v>526</v>
       </c>
       <c r="C139" s="1" t="s">
-        <v>433</v>
+        <v>440</v>
       </c>
       <c r="D139" s="2" t="n">
         <v>2</v>
       </c>
       <c r="F139" s="1" t="s">
-        <v>520</v>
+        <v>527</v>
       </c>
       <c r="H139" s="12" t="s">
-        <v>521</v>
+        <v>528</v>
       </c>
       <c r="I139" s="8" t="s">
-        <v>522</v>
+        <v>529</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5768,22 +5844,22 @@
         <v>132</v>
       </c>
       <c r="B140" s="1" t="s">
-        <v>523</v>
+        <v>530</v>
       </c>
       <c r="C140" s="1" t="s">
-        <v>433</v>
+        <v>440</v>
       </c>
       <c r="D140" s="2" t="n">
         <v>1</v>
       </c>
       <c r="F140" s="1" t="s">
-        <v>524</v>
+        <v>531</v>
       </c>
       <c r="H140" s="7" t="s">
-        <v>525</v>
+        <v>532</v>
       </c>
       <c r="I140" s="7" t="s">
-        <v>526</v>
+        <v>533</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5791,22 +5867,22 @@
         <v>133</v>
       </c>
       <c r="B141" s="1" t="s">
-        <v>527</v>
+        <v>534</v>
       </c>
       <c r="C141" s="1" t="s">
-        <v>478</v>
+        <v>485</v>
       </c>
       <c r="D141" s="2" t="n">
         <v>1</v>
       </c>
       <c r="F141" s="1" t="s">
-        <v>528</v>
+        <v>535</v>
       </c>
       <c r="H141" s="5" t="s">
-        <v>529</v>
+        <v>536</v>
       </c>
       <c r="I141" s="8" t="s">
-        <v>530</v>
+        <v>537</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5814,22 +5890,22 @@
         <v>138</v>
       </c>
       <c r="B142" s="1" t="s">
-        <v>531</v>
+        <v>538</v>
       </c>
       <c r="C142" s="1" t="s">
-        <v>290</v>
+        <v>295</v>
       </c>
       <c r="D142" s="2" t="n">
         <v>1</v>
       </c>
       <c r="F142" s="1" t="s">
-        <v>532</v>
+        <v>539</v>
       </c>
       <c r="H142" s="5" t="s">
-        <v>533</v>
+        <v>540</v>
       </c>
       <c r="I142" s="5" t="s">
-        <v>534</v>
+        <v>541</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5837,22 +5913,22 @@
         <v>141</v>
       </c>
       <c r="B143" s="1" t="s">
-        <v>535</v>
+        <v>542</v>
       </c>
       <c r="C143" s="1" t="s">
-        <v>438</v>
+        <v>445</v>
       </c>
       <c r="D143" s="2" t="n">
         <v>1</v>
       </c>
       <c r="F143" s="1" t="s">
-        <v>536</v>
+        <v>543</v>
       </c>
       <c r="H143" s="5" t="s">
-        <v>537</v>
+        <v>544</v>
       </c>
       <c r="I143" s="5" t="s">
-        <v>538</v>
+        <v>545</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5860,28 +5936,28 @@
         <v>145</v>
       </c>
       <c r="B144" s="1" t="s">
-        <v>539</v>
+        <v>546</v>
       </c>
       <c r="C144" s="1" t="s">
-        <v>478</v>
+        <v>485</v>
       </c>
       <c r="D144" s="2" t="n">
         <v>1</v>
       </c>
       <c r="F144" s="1" t="s">
-        <v>540</v>
+        <v>547</v>
       </c>
       <c r="H144" s="5" t="s">
-        <v>541</v>
+        <v>548</v>
       </c>
       <c r="I144" s="5" t="s">
-        <v>542</v>
+        <v>549</v>
       </c>
       <c r="J144" s="5" t="s">
-        <v>543</v>
+        <v>550</v>
       </c>
       <c r="K144" s="5" t="s">
-        <v>544</v>
+        <v>551</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5902,13 +5978,13 @@
         <v>4</v>
       </c>
       <c r="F146" s="5" t="s">
-        <v>545</v>
+        <v>552</v>
       </c>
       <c r="H146" s="6" t="s">
-        <v>546</v>
+        <v>553</v>
       </c>
       <c r="I146" s="8" t="s">
-        <v>547</v>
+        <v>554</v>
       </c>
       <c r="J146" s="5"/>
     </row>
@@ -5917,13 +5993,13 @@
         <v>2</v>
       </c>
       <c r="F147" s="5" t="s">
-        <v>548</v>
+        <v>555</v>
       </c>
       <c r="H147" s="5" t="s">
-        <v>549</v>
+        <v>556</v>
       </c>
       <c r="I147" s="5" t="s">
-        <v>550</v>
+        <v>557</v>
       </c>
       <c r="J147" s="5"/>
     </row>
@@ -5932,13 +6008,13 @@
         <v>3</v>
       </c>
       <c r="F148" s="5" t="s">
-        <v>551</v>
+        <v>558</v>
       </c>
       <c r="H148" s="5" t="s">
-        <v>552</v>
+        <v>559</v>
       </c>
       <c r="I148" s="5" t="s">
-        <v>553</v>
+        <v>560</v>
       </c>
       <c r="J148" s="5"/>
     </row>
@@ -5947,13 +6023,13 @@
         <v>8</v>
       </c>
       <c r="F149" s="5" t="s">
-        <v>554</v>
+        <v>561</v>
       </c>
       <c r="H149" s="5" t="s">
-        <v>555</v>
+        <v>562</v>
       </c>
       <c r="I149" s="5" t="s">
-        <v>556</v>
+        <v>563</v>
       </c>
       <c r="J149" s="5"/>
     </row>
@@ -5962,19 +6038,19 @@
         <v>11</v>
       </c>
       <c r="F150" s="5" t="s">
-        <v>557</v>
+        <v>564</v>
       </c>
       <c r="H150" s="5" t="s">
-        <v>558</v>
+        <v>565</v>
       </c>
       <c r="I150" s="5" t="s">
-        <v>559</v>
+        <v>566</v>
       </c>
       <c r="J150" s="5" t="s">
-        <v>560</v>
+        <v>567</v>
       </c>
       <c r="K150" s="8" t="s">
-        <v>561</v>
+        <v>568</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5982,13 +6058,13 @@
         <v>5</v>
       </c>
       <c r="F151" s="5" t="s">
-        <v>562</v>
+        <v>569</v>
       </c>
       <c r="H151" s="5" t="s">
-        <v>563</v>
+        <v>570</v>
       </c>
       <c r="I151" s="5" t="s">
-        <v>564</v>
+        <v>571</v>
       </c>
       <c r="J151" s="5"/>
     </row>
@@ -5997,19 +6073,19 @@
         <v>2</v>
       </c>
       <c r="F152" s="5" t="s">
-        <v>565</v>
-      </c>
-      <c r="H152" s="6" t="s">
-        <v>566</v>
-      </c>
-      <c r="I152" s="5" t="s">
-        <v>567</v>
-      </c>
-      <c r="J152" s="5" t="s">
-        <v>568</v>
+        <v>572</v>
+      </c>
+      <c r="H152" s="1" t="s">
+        <v>573</v>
+      </c>
+      <c r="I152" s="1" t="s">
+        <v>574</v>
+      </c>
+      <c r="J152" s="6" t="s">
+        <v>575</v>
       </c>
       <c r="K152" s="5" t="s">
-        <v>569</v>
+        <v>576</v>
       </c>
     </row>
     <row r="153" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6030,22 +6106,22 @@
         <v>98</v>
       </c>
       <c r="B154" s="1" t="s">
-        <v>570</v>
+        <v>577</v>
       </c>
       <c r="C154" s="1" t="s">
-        <v>571</v>
+        <v>578</v>
       </c>
       <c r="D154" s="2" t="n">
         <v>1</v>
       </c>
       <c r="F154" s="1" t="s">
-        <v>571</v>
+        <v>578</v>
       </c>
       <c r="H154" s="5" t="s">
-        <v>572</v>
+        <v>579</v>
       </c>
       <c r="I154" s="5" t="s">
-        <v>573</v>
+        <v>580</v>
       </c>
     </row>
     <row r="155" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6053,22 +6129,22 @@
         <v>16</v>
       </c>
       <c r="B155" s="1" t="s">
-        <v>574</v>
+        <v>581</v>
       </c>
       <c r="C155" s="1" t="s">
-        <v>575</v>
+        <v>582</v>
       </c>
       <c r="D155" s="2" t="n">
         <v>2</v>
       </c>
       <c r="F155" s="1" t="s">
-        <v>576</v>
+        <v>583</v>
       </c>
       <c r="H155" s="5" t="s">
-        <v>577</v>
+        <v>584</v>
       </c>
       <c r="I155" s="5" t="s">
-        <v>578</v>
+        <v>585</v>
       </c>
     </row>
     <row r="156" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6076,10 +6152,10 @@
         <v>60</v>
       </c>
       <c r="B156" s="1" t="s">
-        <v>579</v>
+        <v>586</v>
       </c>
       <c r="C156" s="1" t="s">
-        <v>580</v>
+        <v>587</v>
       </c>
       <c r="D156" s="2" t="n">
         <v>0</v>
@@ -6088,10 +6164,10 @@
         <v>1</v>
       </c>
       <c r="F156" s="1" t="s">
-        <v>581</v>
+        <v>588</v>
       </c>
       <c r="I156" s="1" t="s">
-        <v>582</v>
+        <v>589</v>
       </c>
     </row>
     <row r="157" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6099,22 +6175,22 @@
         <v>82</v>
       </c>
       <c r="B157" s="1" t="s">
-        <v>583</v>
+        <v>590</v>
       </c>
       <c r="C157" s="1" t="s">
-        <v>584</v>
+        <v>591</v>
       </c>
       <c r="D157" s="2" t="n">
         <v>1</v>
       </c>
       <c r="F157" s="1" t="s">
-        <v>585</v>
+        <v>592</v>
       </c>
       <c r="H157" s="5" t="s">
-        <v>586</v>
+        <v>593</v>
       </c>
       <c r="I157" s="5" t="s">
-        <v>587</v>
+        <v>594</v>
       </c>
     </row>
     <row r="158" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6122,19 +6198,19 @@
         <v>83</v>
       </c>
       <c r="B158" s="1" t="s">
-        <v>588</v>
+        <v>595</v>
       </c>
       <c r="C158" s="1" t="s">
-        <v>589</v>
+        <v>596</v>
       </c>
       <c r="D158" s="2" t="n">
         <v>1</v>
       </c>
       <c r="F158" s="1" t="s">
-        <v>590</v>
+        <v>597</v>
       </c>
       <c r="H158" s="5" t="s">
-        <v>591</v>
+        <v>598</v>
       </c>
       <c r="I158" s="5" t="n">
         <v>9282486804791</v>
@@ -6145,10 +6221,10 @@
         <v>94</v>
       </c>
       <c r="B159" s="1" t="s">
-        <v>592</v>
+        <v>599</v>
       </c>
       <c r="C159" s="1" t="s">
-        <v>593</v>
+        <v>600</v>
       </c>
       <c r="D159" s="2" t="n">
         <v>0</v>
@@ -6157,10 +6233,10 @@
         <v>1</v>
       </c>
       <c r="F159" s="1" t="s">
-        <v>594</v>
+        <v>601</v>
       </c>
       <c r="I159" s="1" t="s">
-        <v>582</v>
+        <v>589</v>
       </c>
     </row>
     <row r="160" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6168,22 +6244,22 @@
         <v>99</v>
       </c>
       <c r="B160" s="1" t="s">
-        <v>595</v>
+        <v>602</v>
       </c>
       <c r="C160" s="1" t="s">
-        <v>596</v>
+        <v>603</v>
       </c>
       <c r="D160" s="2" t="n">
         <v>1</v>
       </c>
       <c r="F160" s="1" t="s">
-        <v>596</v>
+        <v>603</v>
       </c>
       <c r="H160" s="5" t="s">
-        <v>597</v>
+        <v>604</v>
       </c>
       <c r="I160" s="5" t="s">
-        <v>598</v>
+        <v>605</v>
       </c>
     </row>
     <row r="161" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6191,22 +6267,22 @@
         <v>102</v>
       </c>
       <c r="B161" s="1" t="s">
-        <v>599</v>
+        <v>606</v>
       </c>
       <c r="C161" s="1" t="s">
-        <v>600</v>
+        <v>607</v>
       </c>
       <c r="D161" s="2" t="n">
         <v>1</v>
       </c>
       <c r="F161" s="1" t="s">
-        <v>600</v>
+        <v>607</v>
       </c>
       <c r="H161" s="5" t="s">
-        <v>601</v>
+        <v>608</v>
       </c>
       <c r="I161" s="5" t="s">
-        <v>602</v>
+        <v>609</v>
       </c>
     </row>
     <row r="162" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6214,22 +6290,22 @@
         <v>115</v>
       </c>
       <c r="B162" s="1" t="s">
-        <v>603</v>
+        <v>610</v>
       </c>
       <c r="C162" s="1" t="s">
-        <v>604</v>
+        <v>611</v>
       </c>
       <c r="D162" s="2" t="n">
         <v>1</v>
       </c>
       <c r="F162" s="1" t="s">
-        <v>605</v>
+        <v>612</v>
       </c>
       <c r="H162" s="5" t="s">
-        <v>606</v>
+        <v>613</v>
       </c>
       <c r="I162" s="5" t="s">
-        <v>607</v>
+        <v>614</v>
       </c>
     </row>
     <row r="163" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6237,10 +6313,10 @@
         <v>121</v>
       </c>
       <c r="B163" s="1" t="s">
-        <v>608</v>
+        <v>615</v>
       </c>
       <c r="C163" s="1" t="s">
-        <v>609</v>
+        <v>616</v>
       </c>
       <c r="D163" s="2" t="n">
         <v>0</v>
@@ -6249,10 +6325,10 @@
         <v>1</v>
       </c>
       <c r="F163" s="1" t="s">
-        <v>610</v>
+        <v>617</v>
       </c>
       <c r="I163" s="1" t="s">
-        <v>582</v>
+        <v>589</v>
       </c>
     </row>
     <row r="164" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6260,28 +6336,28 @@
         <v>144</v>
       </c>
       <c r="B164" s="1" t="s">
-        <v>611</v>
+        <v>618</v>
       </c>
       <c r="C164" s="1" t="s">
-        <v>612</v>
+        <v>619</v>
       </c>
       <c r="D164" s="2" t="n">
         <v>1</v>
       </c>
       <c r="F164" s="1" t="s">
-        <v>613</v>
+        <v>620</v>
       </c>
       <c r="H164" s="5" t="s">
-        <v>614</v>
+        <v>621</v>
       </c>
       <c r="I164" s="5" t="s">
-        <v>615</v>
+        <v>622</v>
       </c>
       <c r="J164" s="5" t="s">
-        <v>616</v>
+        <v>623</v>
       </c>
       <c r="K164" s="5" t="s">
-        <v>617</v>
+        <v>624</v>
       </c>
     </row>
     <row r="165" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6289,28 +6365,28 @@
         <v>156</v>
       </c>
       <c r="B165" s="1" t="s">
-        <v>618</v>
+        <v>625</v>
       </c>
       <c r="C165" s="1" t="s">
-        <v>619</v>
+        <v>626</v>
       </c>
       <c r="D165" s="2" t="n">
         <v>1</v>
       </c>
       <c r="F165" s="1" t="s">
-        <v>620</v>
+        <v>627</v>
       </c>
       <c r="H165" s="1" t="s">
-        <v>621</v>
+        <v>628</v>
       </c>
       <c r="I165" s="1" t="n">
         <v>9032646824</v>
       </c>
       <c r="J165" s="5" t="s">
-        <v>622</v>
+        <v>629</v>
       </c>
       <c r="K165" s="5" t="s">
-        <v>623</v>
+        <v>630</v>
       </c>
     </row>
     <row r="166" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6331,22 +6407,22 @@
         <v>23</v>
       </c>
       <c r="B167" s="1" t="s">
-        <v>624</v>
+        <v>631</v>
       </c>
       <c r="C167" s="1" t="s">
-        <v>625</v>
+        <v>632</v>
       </c>
       <c r="D167" s="2" t="n">
         <v>2</v>
       </c>
       <c r="F167" s="1" t="s">
-        <v>626</v>
+        <v>633</v>
       </c>
       <c r="H167" s="5" t="s">
-        <v>627</v>
+        <v>634</v>
       </c>
       <c r="I167" s="5" t="s">
-        <v>628</v>
+        <v>635</v>
       </c>
     </row>
     <row r="168" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6354,13 +6430,13 @@
         <v>1</v>
       </c>
       <c r="F168" s="1" t="s">
-        <v>629</v>
+        <v>636</v>
       </c>
       <c r="H168" s="5" t="s">
-        <v>630</v>
+        <v>637</v>
       </c>
       <c r="I168" s="5" t="s">
-        <v>631</v>
+        <v>638</v>
       </c>
     </row>
     <row r="169" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6368,49 +6444,49 @@
         <v>37</v>
       </c>
       <c r="B169" s="1" t="s">
-        <v>632</v>
+        <v>639</v>
       </c>
       <c r="C169" s="1" t="s">
-        <v>633</v>
+        <v>640</v>
       </c>
       <c r="D169" s="2" t="n">
         <v>12</v>
       </c>
       <c r="F169" s="1" t="s">
-        <v>634</v>
+        <v>641</v>
       </c>
       <c r="H169" s="5" t="s">
-        <v>635</v>
+        <v>642</v>
       </c>
       <c r="I169" s="5" t="s">
-        <v>636</v>
+        <v>643</v>
       </c>
       <c r="J169" s="5" t="s">
-        <v>637</v>
+        <v>644</v>
       </c>
       <c r="K169" s="5" t="s">
-        <v>638</v>
+        <v>645</v>
       </c>
     </row>
     <row r="170" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B170" s="1" t="s">
-        <v>639</v>
+        <v>646</v>
       </c>
       <c r="C170" s="1" t="s">
-        <v>640</v>
+        <v>647</v>
       </c>
       <c r="D170" s="2" t="n">
         <v>32</v>
       </c>
       <c r="E170" s="1"/>
       <c r="F170" s="1" t="s">
-        <v>641</v>
+        <v>648</v>
       </c>
       <c r="H170" s="1" t="s">
-        <v>642</v>
+        <v>649</v>
       </c>
       <c r="I170" s="1" t="s">
-        <v>643</v>
+        <v>650</v>
       </c>
     </row>
     <row r="171" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6418,22 +6494,22 @@
         <v>91</v>
       </c>
       <c r="B171" s="1" t="s">
-        <v>644</v>
+        <v>651</v>
       </c>
       <c r="C171" s="1" t="s">
-        <v>645</v>
+        <v>652</v>
       </c>
       <c r="D171" s="2" t="n">
         <v>1</v>
       </c>
       <c r="F171" s="1" t="s">
-        <v>646</v>
+        <v>653</v>
       </c>
       <c r="H171" s="7" t="s">
-        <v>647</v>
+        <v>654</v>
       </c>
       <c r="I171" s="7" t="s">
-        <v>648</v>
+        <v>655</v>
       </c>
     </row>
     <row r="172" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6441,22 +6517,22 @@
         <v>87</v>
       </c>
       <c r="B172" s="1" t="s">
-        <v>649</v>
+        <v>656</v>
       </c>
       <c r="C172" s="1" t="s">
-        <v>650</v>
+        <v>657</v>
       </c>
       <c r="D172" s="2" t="n">
         <v>1</v>
       </c>
       <c r="F172" s="1" t="s">
-        <v>651</v>
+        <v>658</v>
       </c>
       <c r="H172" s="5" t="s">
-        <v>652</v>
+        <v>659</v>
       </c>
       <c r="I172" s="5" t="s">
-        <v>653</v>
+        <v>660</v>
       </c>
     </row>
     <row r="173" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6477,22 +6553,22 @@
         <v>27</v>
       </c>
       <c r="B174" s="1" t="s">
-        <v>654</v>
+        <v>661</v>
       </c>
       <c r="C174" s="1" t="s">
-        <v>655</v>
+        <v>662</v>
       </c>
       <c r="D174" s="2" t="n">
         <v>2</v>
       </c>
       <c r="F174" s="1" t="s">
-        <v>656</v>
+        <v>663</v>
       </c>
       <c r="H174" s="7" t="s">
-        <v>657</v>
+        <v>664</v>
       </c>
       <c r="I174" s="7" t="s">
-        <v>658</v>
+        <v>665</v>
       </c>
     </row>
     <row r="175" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6500,28 +6576,28 @@
         <v>126</v>
       </c>
       <c r="B175" s="1" t="s">
-        <v>659</v>
+        <v>666</v>
       </c>
       <c r="C175" s="1" t="s">
-        <v>660</v>
+        <v>667</v>
       </c>
       <c r="D175" s="2" t="n">
         <v>1</v>
       </c>
       <c r="F175" s="1" t="s">
-        <v>661</v>
+        <v>668</v>
       </c>
       <c r="H175" s="1" t="s">
-        <v>662</v>
+        <v>669</v>
       </c>
       <c r="I175" s="1" t="s">
-        <v>663</v>
+        <v>670</v>
       </c>
       <c r="J175" s="1" t="s">
-        <v>664</v>
+        <v>671</v>
       </c>
       <c r="K175" s="1" t="s">
-        <v>665</v>
+        <v>672</v>
       </c>
     </row>
     <row r="176" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6542,22 +6618,22 @@
         <v>48</v>
       </c>
       <c r="B177" s="1" t="s">
-        <v>666</v>
+        <v>673</v>
       </c>
       <c r="C177" s="1" t="s">
-        <v>667</v>
+        <v>674</v>
       </c>
       <c r="D177" s="2" t="n">
         <v>1</v>
       </c>
       <c r="F177" s="1" t="s">
-        <v>668</v>
+        <v>675</v>
       </c>
       <c r="H177" s="5" t="s">
-        <v>669</v>
+        <v>676</v>
       </c>
       <c r="I177" s="8" t="s">
-        <v>670</v>
+        <v>677</v>
       </c>
     </row>
     <row r="178" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6565,68 +6641,73 @@
         <v>69</v>
       </c>
       <c r="B178" s="1" t="s">
-        <v>671</v>
+        <v>678</v>
       </c>
       <c r="C178" s="1" t="s">
-        <v>672</v>
+        <v>679</v>
       </c>
       <c r="D178" s="2" t="n">
         <v>1</v>
       </c>
       <c r="F178" s="1" t="s">
-        <v>673</v>
+        <v>680</v>
       </c>
       <c r="H178" s="7" t="s">
-        <v>674</v>
+        <v>681</v>
       </c>
       <c r="I178" s="7" t="s">
-        <v>675</v>
-      </c>
-    </row>
-    <row r="179" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>682</v>
+      </c>
+    </row>
+    <row r="179" s="13" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A179" s="1" t="n">
         <v>79</v>
       </c>
       <c r="B179" s="1" t="s">
-        <v>676</v>
+        <v>683</v>
       </c>
       <c r="C179" s="1" t="s">
-        <v>677</v>
+        <v>684</v>
       </c>
       <c r="D179" s="2" t="n">
         <v>1</v>
       </c>
+      <c r="E179" s="2"/>
       <c r="F179" s="1" t="s">
-        <v>678</v>
-      </c>
+        <v>685</v>
+      </c>
+      <c r="G179" s="1"/>
       <c r="H179" s="7" t="s">
-        <v>679</v>
+        <v>686</v>
       </c>
       <c r="I179" s="7" t="s">
-        <v>680</v>
-      </c>
+        <v>687</v>
+      </c>
+      <c r="J179" s="1"/>
+      <c r="K179" s="1"/>
+      <c r="L179" s="1"/>
     </row>
     <row r="180" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A180" s="1" t="n">
         <v>136</v>
       </c>
       <c r="B180" s="1" t="s">
-        <v>681</v>
+        <v>688</v>
       </c>
       <c r="C180" s="1" t="s">
-        <v>682</v>
+        <v>689</v>
       </c>
       <c r="D180" s="2" t="n">
         <v>1</v>
       </c>
       <c r="F180" s="1" t="s">
-        <v>683</v>
+        <v>690</v>
       </c>
       <c r="H180" s="5" t="s">
-        <v>684</v>
+        <v>691</v>
       </c>
       <c r="I180" s="5" t="s">
-        <v>685</v>
+        <v>692</v>
       </c>
     </row>
     <row r="181" s="13" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6634,10 +6715,10 @@
         <v>149</v>
       </c>
       <c r="B181" s="13" t="s">
-        <v>686</v>
+        <v>693</v>
       </c>
       <c r="C181" s="13" t="s">
-        <v>667</v>
+        <v>674</v>
       </c>
       <c r="D181" s="2" t="n">
         <v>0</v>
@@ -6646,19 +6727,19 @@
         <v>1</v>
       </c>
       <c r="F181" s="13" t="s">
-        <v>687</v>
+        <v>694</v>
       </c>
       <c r="H181" s="15" t="s">
-        <v>688</v>
+        <v>695</v>
       </c>
       <c r="I181" s="15" t="s">
-        <v>689</v>
+        <v>696</v>
       </c>
       <c r="J181" s="15" t="s">
-        <v>690</v>
+        <v>697</v>
       </c>
       <c r="K181" s="15" t="s">
-        <v>691</v>
+        <v>698</v>
       </c>
       <c r="L181" s="1"/>
     </row>
@@ -6675,15 +6756,15 @@
       <c r="J182" s="3"/>
       <c r="K182" s="3"/>
     </row>
-    <row r="183" s="13" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="183" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A183" s="13" t="n">
         <v>89</v>
       </c>
       <c r="B183" s="13" t="s">
-        <v>692</v>
+        <v>699</v>
       </c>
       <c r="C183" s="13" t="s">
-        <v>693</v>
+        <v>700</v>
       </c>
       <c r="D183" s="2" t="n">
         <v>0</v>
@@ -6692,28 +6773,30 @@
         <v>1</v>
       </c>
       <c r="F183" s="13" t="s">
-        <v>694</v>
-      </c>
+        <v>701</v>
+      </c>
+      <c r="G183" s="13"/>
       <c r="H183" s="13" t="s">
-        <v>695</v>
+        <v>702</v>
       </c>
       <c r="I183" s="13" t="s">
-        <v>696</v>
-      </c>
-      <c r="L183" s="1"/>
+        <v>703</v>
+      </c>
+      <c r="J183" s="13"/>
+      <c r="K183" s="13"/>
     </row>
     <row r="184" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D184" s="2" t="n">
         <v>1</v>
       </c>
       <c r="F184" s="5" t="s">
-        <v>697</v>
+        <v>704</v>
       </c>
       <c r="H184" s="5" t="s">
-        <v>698</v>
+        <v>705</v>
       </c>
       <c r="I184" s="5" t="s">
-        <v>699</v>
+        <v>706</v>
       </c>
     </row>
     <row r="185" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6721,22 +6804,22 @@
         <v>122</v>
       </c>
       <c r="B185" s="1" t="s">
-        <v>700</v>
+        <v>707</v>
       </c>
       <c r="C185" s="1" t="s">
-        <v>701</v>
+        <v>708</v>
       </c>
       <c r="D185" s="2" t="n">
         <v>1</v>
       </c>
       <c r="F185" s="1" t="s">
-        <v>702</v>
+        <v>709</v>
       </c>
       <c r="H185" s="5" t="s">
-        <v>703</v>
+        <v>710</v>
       </c>
       <c r="I185" s="5" t="s">
-        <v>704</v>
+        <v>711</v>
       </c>
     </row>
     <row r="186" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6744,19 +6827,19 @@
         <v>2</v>
       </c>
       <c r="F186" s="5" t="s">
-        <v>697</v>
+        <v>704</v>
       </c>
       <c r="H186" s="1" t="s">
-        <v>705</v>
+        <v>712</v>
       </c>
       <c r="I186" s="1" t="s">
-        <v>706</v>
+        <v>713</v>
       </c>
       <c r="J186" s="7" t="s">
-        <v>707</v>
+        <v>714</v>
       </c>
       <c r="K186" s="7" t="s">
-        <v>708</v>
+        <v>715</v>
       </c>
     </row>
     <row r="187" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6764,22 +6847,22 @@
         <v>154</v>
       </c>
       <c r="B187" s="1" t="s">
-        <v>709</v>
+        <v>716</v>
       </c>
       <c r="C187" s="1" t="s">
-        <v>710</v>
+        <v>717</v>
       </c>
       <c r="D187" s="2" t="n">
         <v>1</v>
       </c>
       <c r="F187" s="1" t="s">
-        <v>711</v>
+        <v>718</v>
       </c>
       <c r="H187" s="7" t="s">
-        <v>712</v>
+        <v>719</v>
       </c>
       <c r="I187" s="7" t="s">
-        <v>713</v>
+        <v>720</v>
       </c>
     </row>
     <row r="188" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6787,22 +6870,22 @@
         <v>155</v>
       </c>
       <c r="B188" s="1" t="s">
-        <v>714</v>
+        <v>721</v>
       </c>
       <c r="C188" s="1" t="s">
-        <v>715</v>
+        <v>722</v>
       </c>
       <c r="D188" s="2" t="n">
         <v>1</v>
       </c>
       <c r="F188" s="1" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
       <c r="H188" s="7" t="s">
-        <v>716</v>
+        <v>723</v>
       </c>
       <c r="I188" s="7" t="s">
-        <v>717</v>
+        <v>724</v>
       </c>
     </row>
     <row r="189" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6810,13 +6893,13 @@
         <v>1</v>
       </c>
       <c r="F189" s="5" t="s">
-        <v>697</v>
+        <v>704</v>
       </c>
       <c r="H189" s="7" t="s">
-        <v>718</v>
+        <v>725</v>
       </c>
       <c r="I189" s="7" t="s">
-        <v>719</v>
+        <v>726</v>
       </c>
     </row>
     <row r="190" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6834,13 +6917,13 @@
     </row>
     <row r="192" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B192" s="1" t="s">
-        <v>720</v>
+        <v>727</v>
       </c>
       <c r="D192" s="2" t="n">
         <v>3</v>
       </c>
       <c r="H192" s="1" t="s">
-        <v>721</v>
+        <v>728</v>
       </c>
       <c r="I192" s="16" t="n">
         <v>830207670409</v>
@@ -6848,30 +6931,41 @@
     </row>
     <row r="193" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B193" s="1" t="s">
-        <v>722</v>
+        <v>729</v>
       </c>
       <c r="D193" s="2" t="n">
         <v>2</v>
       </c>
       <c r="H193" s="1" t="s">
-        <v>723</v>
+        <v>730</v>
       </c>
       <c r="I193" s="1" t="s">
-        <v>724</v>
+        <v>731</v>
       </c>
     </row>
     <row r="194" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B194" s="1" t="s">
-        <v>722</v>
+        <v>729</v>
       </c>
       <c r="D194" s="2" t="n">
         <v>2</v>
       </c>
       <c r="H194" s="1" t="s">
-        <v>725</v>
+        <v>732</v>
       </c>
       <c r="I194" s="1" t="s">
-        <v>726</v>
+        <v>733</v>
+      </c>
+    </row>
+    <row r="196" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B196" s="1" t="s">
+        <v>734</v>
+      </c>
+      <c r="H196" s="1" t="s">
+        <v>735</v>
+      </c>
+      <c r="I196" s="1" t="s">
+        <v>736</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix boms, audio connector footprint
</commit_message>
<xml_diff>
--- a/Board/bom/cbm_ultipet_v1.2a-bom.xlsx
+++ b/Board/bom/cbm_ultipet_v1.2a-bom.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="883" uniqueCount="737">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="878" uniqueCount="733">
   <si>
     <t xml:space="preserve">Id</t>
   </si>
@@ -1609,18 +1609,6 @@
   </si>
   <si>
     <t xml:space="preserve">74HCT00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TQFP-48_7x7mm_P0.5mm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TL16C752C</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 595-TL16C752DPFBR </t>
-  </si>
-  <si>
-    <t xml:space="preserve">TL16C752DPFBR </t>
   </si>
   <si>
     <t xml:space="preserve">IC49</t>
@@ -2637,14 +2625,14 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L196"/>
+  <dimension ref="A1:L195"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B164" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B119" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A164" activeCellId="0" sqref="A164"/>
-      <selection pane="bottomRight" activeCell="B196" activeCellId="0" sqref="B196:I196"/>
+      <selection pane="bottomLeft" activeCell="A119" activeCellId="0" sqref="A119"/>
+      <selection pane="bottomRight" activeCell="B137" activeCellId="0" sqref="B137"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5772,13 +5760,13 @@
     </row>
     <row r="137" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="1" t="n">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B137" s="1" t="s">
-        <v>444</v>
+        <v>518</v>
       </c>
       <c r="C137" s="1" t="s">
-        <v>518</v>
+        <v>476</v>
       </c>
       <c r="D137" s="2" t="n">
         <v>1</v>
@@ -5795,30 +5783,30 @@
     </row>
     <row r="138" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="1" t="n">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="B138" s="1" t="s">
         <v>522</v>
       </c>
       <c r="C138" s="1" t="s">
-        <v>476</v>
+        <v>440</v>
       </c>
       <c r="D138" s="2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F138" s="1" t="s">
         <v>523</v>
       </c>
-      <c r="H138" s="5" t="s">
+      <c r="H138" s="12" t="s">
         <v>524</v>
       </c>
-      <c r="I138" s="5" t="s">
+      <c r="I138" s="8" t="s">
         <v>525</v>
       </c>
     </row>
-    <row r="139" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="139" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="1" t="n">
-        <v>127</v>
+        <v>132</v>
       </c>
       <c r="B139" s="1" t="s">
         <v>526</v>
@@ -5827,27 +5815,27 @@
         <v>440</v>
       </c>
       <c r="D139" s="2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F139" s="1" t="s">
         <v>527</v>
       </c>
-      <c r="H139" s="12" t="s">
+      <c r="H139" s="7" t="s">
         <v>528</v>
       </c>
-      <c r="I139" s="8" t="s">
+      <c r="I139" s="7" t="s">
         <v>529</v>
       </c>
     </row>
-    <row r="140" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="140" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="1" t="n">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B140" s="1" t="s">
         <v>530</v>
       </c>
       <c r="C140" s="1" t="s">
-        <v>440</v>
+        <v>485</v>
       </c>
       <c r="D140" s="2" t="n">
         <v>1</v>
@@ -5855,22 +5843,22 @@
       <c r="F140" s="1" t="s">
         <v>531</v>
       </c>
-      <c r="H140" s="7" t="s">
+      <c r="H140" s="5" t="s">
         <v>532</v>
       </c>
-      <c r="I140" s="7" t="s">
+      <c r="I140" s="8" t="s">
         <v>533</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="1" t="n">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="B141" s="1" t="s">
         <v>534</v>
       </c>
       <c r="C141" s="1" t="s">
-        <v>485</v>
+        <v>295</v>
       </c>
       <c r="D141" s="2" t="n">
         <v>1</v>
@@ -5881,19 +5869,19 @@
       <c r="H141" s="5" t="s">
         <v>536</v>
       </c>
-      <c r="I141" s="8" t="s">
+      <c r="I141" s="5" t="s">
         <v>537</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="1" t="n">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="B142" s="1" t="s">
         <v>538</v>
       </c>
       <c r="C142" s="1" t="s">
-        <v>295</v>
+        <v>445</v>
       </c>
       <c r="D142" s="2" t="n">
         <v>1</v>
@@ -5910,13 +5898,13 @@
     </row>
     <row r="143" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="1" t="n">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="B143" s="1" t="s">
         <v>542</v>
       </c>
       <c r="C143" s="1" t="s">
-        <v>445</v>
+        <v>485</v>
       </c>
       <c r="D143" s="2" t="n">
         <v>1</v>
@@ -5930,180 +5918,180 @@
       <c r="I143" s="5" t="s">
         <v>545</v>
       </c>
+      <c r="J143" s="5" t="s">
+        <v>546</v>
+      </c>
+      <c r="K143" s="5" t="s">
+        <v>547</v>
+      </c>
     </row>
     <row r="144" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A144" s="1" t="n">
-        <v>145</v>
-      </c>
-      <c r="B144" s="1" t="s">
-        <v>546</v>
-      </c>
-      <c r="C144" s="1" t="s">
-        <v>485</v>
-      </c>
-      <c r="D144" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="F144" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="H144" s="5" t="s">
+      <c r="A144" s="3"/>
+      <c r="B144" s="3"/>
+      <c r="C144" s="3"/>
+      <c r="D144" s="4"/>
+      <c r="E144" s="4"/>
+      <c r="F144" s="3"/>
+      <c r="G144" s="3"/>
+      <c r="H144" s="3"/>
+      <c r="I144" s="3"/>
+      <c r="J144" s="3"/>
+      <c r="K144" s="3"/>
+    </row>
+    <row r="145" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D145" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="F145" s="5" t="s">
         <v>548</v>
       </c>
-      <c r="I144" s="5" t="s">
+      <c r="H145" s="6" t="s">
         <v>549</v>
       </c>
-      <c r="J144" s="5" t="s">
+      <c r="I145" s="8" t="s">
         <v>550</v>
       </c>
-      <c r="K144" s="5" t="s">
-        <v>551</v>
-      </c>
-    </row>
-    <row r="145" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A145" s="3"/>
-      <c r="B145" s="3"/>
-      <c r="C145" s="3"/>
-      <c r="D145" s="4"/>
-      <c r="E145" s="4"/>
-      <c r="F145" s="3"/>
-      <c r="G145" s="3"/>
-      <c r="H145" s="3"/>
-      <c r="I145" s="3"/>
-      <c r="J145" s="3"/>
-      <c r="K145" s="3"/>
+      <c r="J145" s="5"/>
     </row>
     <row r="146" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D146" s="2" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F146" s="5" t="s">
+        <v>551</v>
+      </c>
+      <c r="H146" s="5" t="s">
         <v>552</v>
       </c>
-      <c r="H146" s="6" t="s">
+      <c r="I146" s="5" t="s">
         <v>553</v>
-      </c>
-      <c r="I146" s="8" t="s">
-        <v>554</v>
       </c>
       <c r="J146" s="5"/>
     </row>
     <row r="147" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D147" s="2" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F147" s="5" t="s">
+        <v>554</v>
+      </c>
+      <c r="H147" s="5" t="s">
         <v>555</v>
       </c>
-      <c r="H147" s="5" t="s">
+      <c r="I147" s="5" t="s">
         <v>556</v>
-      </c>
-      <c r="I147" s="5" t="s">
-        <v>557</v>
       </c>
       <c r="J147" s="5"/>
     </row>
     <row r="148" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D148" s="2" t="n">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="F148" s="5" t="s">
+        <v>557</v>
+      </c>
+      <c r="H148" s="5" t="s">
         <v>558</v>
       </c>
-      <c r="H148" s="5" t="s">
+      <c r="I148" s="5" t="s">
         <v>559</v>
-      </c>
-      <c r="I148" s="5" t="s">
-        <v>560</v>
       </c>
       <c r="J148" s="5"/>
     </row>
     <row r="149" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D149" s="2" t="n">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="F149" s="5" t="s">
+        <v>560</v>
+      </c>
+      <c r="H149" s="5" t="s">
         <v>561</v>
       </c>
-      <c r="H149" s="5" t="s">
+      <c r="I149" s="5" t="s">
         <v>562</v>
       </c>
-      <c r="I149" s="5" t="s">
+      <c r="J149" s="5" t="s">
         <v>563</v>
       </c>
-      <c r="J149" s="5"/>
+      <c r="K149" s="8" t="s">
+        <v>564</v>
+      </c>
     </row>
     <row r="150" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D150" s="2" t="n">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="F150" s="5" t="s">
-        <v>564</v>
+        <v>565</v>
       </c>
       <c r="H150" s="5" t="s">
-        <v>565</v>
+        <v>566</v>
       </c>
       <c r="I150" s="5" t="s">
-        <v>566</v>
-      </c>
-      <c r="J150" s="5" t="s">
         <v>567</v>
       </c>
-      <c r="K150" s="8" t="s">
-        <v>568</v>
-      </c>
+      <c r="J150" s="5"/>
     </row>
     <row r="151" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D151" s="2" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F151" s="5" t="s">
+        <v>568</v>
+      </c>
+      <c r="H151" s="1" t="s">
         <v>569</v>
       </c>
-      <c r="H151" s="5" t="s">
+      <c r="I151" s="1" t="s">
         <v>570</v>
       </c>
-      <c r="I151" s="5" t="s">
+      <c r="J151" s="6" t="s">
         <v>571</v>
       </c>
-      <c r="J151" s="5"/>
+      <c r="K151" s="5" t="s">
+        <v>572</v>
+      </c>
     </row>
     <row r="152" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D152" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="F152" s="5" t="s">
-        <v>572</v>
-      </c>
-      <c r="H152" s="1" t="s">
+      <c r="A152" s="3"/>
+      <c r="B152" s="3"/>
+      <c r="C152" s="3"/>
+      <c r="D152" s="4"/>
+      <c r="E152" s="4"/>
+      <c r="F152" s="3"/>
+      <c r="G152" s="3"/>
+      <c r="H152" s="3"/>
+      <c r="I152" s="3"/>
+      <c r="J152" s="3"/>
+      <c r="K152" s="3"/>
+    </row>
+    <row r="153" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A153" s="1" t="n">
+        <v>98</v>
+      </c>
+      <c r="B153" s="1" t="s">
         <v>573</v>
       </c>
-      <c r="I152" s="1" t="s">
+      <c r="C153" s="1" t="s">
         <v>574</v>
       </c>
-      <c r="J152" s="6" t="s">
+      <c r="D153" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="F153" s="1" t="s">
+        <v>574</v>
+      </c>
+      <c r="H153" s="5" t="s">
         <v>575</v>
       </c>
-      <c r="K152" s="5" t="s">
+      <c r="I153" s="5" t="s">
         <v>576</v>
       </c>
-    </row>
-    <row r="153" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A153" s="3"/>
-      <c r="B153" s="3"/>
-      <c r="C153" s="3"/>
-      <c r="D153" s="4"/>
-      <c r="E153" s="4"/>
-      <c r="F153" s="3"/>
-      <c r="G153" s="3"/>
-      <c r="H153" s="3"/>
-      <c r="I153" s="3"/>
-      <c r="J153" s="3"/>
-      <c r="K153" s="3"/>
     </row>
     <row r="154" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="1" t="n">
-        <v>98</v>
+        <v>16</v>
       </c>
       <c r="B154" s="1" t="s">
         <v>577</v>
@@ -6112,44 +6100,44 @@
         <v>578</v>
       </c>
       <c r="D154" s="2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F154" s="1" t="s">
-        <v>578</v>
+        <v>579</v>
       </c>
       <c r="H154" s="5" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="I154" s="5" t="s">
-        <v>580</v>
+        <v>581</v>
       </c>
     </row>
     <row r="155" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A155" s="1" t="n">
-        <v>16</v>
+        <v>60</v>
       </c>
       <c r="B155" s="1" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="C155" s="1" t="s">
-        <v>582</v>
+        <v>583</v>
       </c>
       <c r="D155" s="2" t="n">
-        <v>2</v>
+        <v>0</v>
+      </c>
+      <c r="E155" s="2" t="n">
+        <v>1</v>
       </c>
       <c r="F155" s="1" t="s">
-        <v>583</v>
-      </c>
-      <c r="H155" s="5" t="s">
         <v>584</v>
       </c>
-      <c r="I155" s="5" t="s">
+      <c r="I155" s="1" t="s">
         <v>585</v>
       </c>
     </row>
     <row r="156" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A156" s="1" t="n">
-        <v>60</v>
+        <v>82</v>
       </c>
       <c r="B156" s="1" t="s">
         <v>586</v>
@@ -6158,44 +6146,44 @@
         <v>587</v>
       </c>
       <c r="D156" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E156" s="2" t="n">
         <v>1</v>
       </c>
       <c r="F156" s="1" t="s">
         <v>588</v>
       </c>
-      <c r="I156" s="1" t="s">
+      <c r="H156" s="5" t="s">
         <v>589</v>
+      </c>
+      <c r="I156" s="5" t="s">
+        <v>590</v>
       </c>
     </row>
     <row r="157" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A157" s="1" t="n">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B157" s="1" t="s">
-        <v>590</v>
+        <v>591</v>
       </c>
       <c r="C157" s="1" t="s">
-        <v>591</v>
+        <v>592</v>
       </c>
       <c r="D157" s="2" t="n">
         <v>1</v>
       </c>
       <c r="F157" s="1" t="s">
-        <v>592</v>
+        <v>593</v>
       </c>
       <c r="H157" s="5" t="s">
-        <v>593</v>
-      </c>
-      <c r="I157" s="5" t="s">
         <v>594</v>
+      </c>
+      <c r="I157" s="5" t="n">
+        <v>9282486804791</v>
       </c>
     </row>
     <row r="158" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A158" s="1" t="n">
-        <v>83</v>
+        <v>94</v>
       </c>
       <c r="B158" s="1" t="s">
         <v>595</v>
@@ -6204,44 +6192,44 @@
         <v>596</v>
       </c>
       <c r="D158" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E158" s="2" t="n">
         <v>1</v>
       </c>
       <c r="F158" s="1" t="s">
         <v>597</v>
       </c>
-      <c r="H158" s="5" t="s">
-        <v>598</v>
-      </c>
-      <c r="I158" s="5" t="n">
-        <v>9282486804791</v>
+      <c r="I158" s="1" t="s">
+        <v>585</v>
       </c>
     </row>
     <row r="159" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A159" s="1" t="n">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="B159" s="1" t="s">
+        <v>598</v>
+      </c>
+      <c r="C159" s="1" t="s">
         <v>599</v>
       </c>
-      <c r="C159" s="1" t="s">
+      <c r="D159" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="F159" s="1" t="s">
+        <v>599</v>
+      </c>
+      <c r="H159" s="5" t="s">
         <v>600</v>
       </c>
-      <c r="D159" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E159" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="F159" s="1" t="s">
+      <c r="I159" s="5" t="s">
         <v>601</v>
-      </c>
-      <c r="I159" s="1" t="s">
-        <v>589</v>
       </c>
     </row>
     <row r="160" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="1" t="n">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="B160" s="1" t="s">
         <v>602</v>
@@ -6264,7 +6252,7 @@
     </row>
     <row r="161" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A161" s="1" t="n">
-        <v>102</v>
+        <v>115</v>
       </c>
       <c r="B161" s="1" t="s">
         <v>606</v>
@@ -6276,587 +6264,587 @@
         <v>1</v>
       </c>
       <c r="F161" s="1" t="s">
-        <v>607</v>
+        <v>608</v>
       </c>
       <c r="H161" s="5" t="s">
-        <v>608</v>
+        <v>609</v>
       </c>
       <c r="I161" s="5" t="s">
-        <v>609</v>
+        <v>610</v>
       </c>
     </row>
     <row r="162" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A162" s="1" t="n">
-        <v>115</v>
+        <v>121</v>
       </c>
       <c r="B162" s="1" t="s">
-        <v>610</v>
+        <v>611</v>
       </c>
       <c r="C162" s="1" t="s">
-        <v>611</v>
+        <v>612</v>
       </c>
       <c r="D162" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E162" s="2" t="n">
         <v>1</v>
       </c>
       <c r="F162" s="1" t="s">
-        <v>612</v>
-      </c>
-      <c r="H162" s="5" t="s">
         <v>613</v>
       </c>
-      <c r="I162" s="5" t="s">
-        <v>614</v>
+      <c r="I162" s="1" t="s">
+        <v>585</v>
       </c>
     </row>
     <row r="163" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A163" s="1" t="n">
-        <v>121</v>
+        <v>144</v>
       </c>
       <c r="B163" s="1" t="s">
+        <v>614</v>
+      </c>
+      <c r="C163" s="1" t="s">
         <v>615</v>
       </c>
-      <c r="C163" s="1" t="s">
+      <c r="D163" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="F163" s="1" t="s">
         <v>616</v>
       </c>
-      <c r="D163" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E163" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="F163" s="1" t="s">
+      <c r="H163" s="5" t="s">
         <v>617</v>
       </c>
-      <c r="I163" s="1" t="s">
-        <v>589</v>
+      <c r="I163" s="5" t="s">
+        <v>618</v>
+      </c>
+      <c r="J163" s="5" t="s">
+        <v>619</v>
+      </c>
+      <c r="K163" s="5" t="s">
+        <v>620</v>
       </c>
     </row>
     <row r="164" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A164" s="1" t="n">
-        <v>144</v>
+        <v>156</v>
       </c>
       <c r="B164" s="1" t="s">
-        <v>618</v>
+        <v>621</v>
       </c>
       <c r="C164" s="1" t="s">
-        <v>619</v>
+        <v>622</v>
       </c>
       <c r="D164" s="2" t="n">
         <v>1</v>
       </c>
       <c r="F164" s="1" t="s">
-        <v>620</v>
-      </c>
-      <c r="H164" s="5" t="s">
-        <v>621</v>
-      </c>
-      <c r="I164" s="5" t="s">
-        <v>622</v>
+        <v>623</v>
+      </c>
+      <c r="H164" s="1" t="s">
+        <v>624</v>
+      </c>
+      <c r="I164" s="1" t="n">
+        <v>9032646824</v>
       </c>
       <c r="J164" s="5" t="s">
-        <v>623</v>
+        <v>625</v>
       </c>
       <c r="K164" s="5" t="s">
-        <v>624</v>
+        <v>626</v>
       </c>
     </row>
     <row r="165" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A165" s="1" t="n">
-        <v>156</v>
-      </c>
-      <c r="B165" s="1" t="s">
-        <v>625</v>
-      </c>
-      <c r="C165" s="1" t="s">
-        <v>626</v>
-      </c>
-      <c r="D165" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="F165" s="1" t="s">
+      <c r="A165" s="3"/>
+      <c r="B165" s="3"/>
+      <c r="C165" s="3"/>
+      <c r="D165" s="4"/>
+      <c r="E165" s="4"/>
+      <c r="F165" s="3"/>
+      <c r="G165" s="3"/>
+      <c r="H165" s="3"/>
+      <c r="I165" s="3"/>
+      <c r="J165" s="3"/>
+      <c r="K165" s="3"/>
+    </row>
+    <row r="166" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A166" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="B166" s="1" t="s">
         <v>627</v>
       </c>
-      <c r="H165" s="1" t="s">
+      <c r="C166" s="1" t="s">
         <v>628</v>
       </c>
-      <c r="I165" s="1" t="n">
-        <v>9032646824</v>
-      </c>
-      <c r="J165" s="5" t="s">
+      <c r="D166" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="F166" s="1" t="s">
         <v>629</v>
       </c>
-      <c r="K165" s="5" t="s">
+      <c r="H166" s="5" t="s">
         <v>630</v>
       </c>
-    </row>
-    <row r="166" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A166" s="3"/>
-      <c r="B166" s="3"/>
-      <c r="C166" s="3"/>
-      <c r="D166" s="4"/>
-      <c r="E166" s="4"/>
-      <c r="F166" s="3"/>
-      <c r="G166" s="3"/>
-      <c r="H166" s="3"/>
-      <c r="I166" s="3"/>
-      <c r="J166" s="3"/>
-      <c r="K166" s="3"/>
+      <c r="I166" s="5" t="s">
+        <v>631</v>
+      </c>
     </row>
     <row r="167" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A167" s="1" t="n">
-        <v>23</v>
-      </c>
-      <c r="B167" s="1" t="s">
-        <v>631</v>
-      </c>
-      <c r="C167" s="1" t="s">
+      <c r="D167" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="F167" s="1" t="s">
         <v>632</v>
       </c>
-      <c r="D167" s="2" t="n">
+      <c r="H167" s="5" t="s">
+        <v>633</v>
+      </c>
+      <c r="I167" s="5" t="s">
+        <v>634</v>
+      </c>
+    </row>
+    <row r="168" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A168" s="1" t="n">
+        <v>37</v>
+      </c>
+      <c r="B168" s="1" t="s">
+        <v>635</v>
+      </c>
+      <c r="C168" s="1" t="s">
+        <v>636</v>
+      </c>
+      <c r="D168" s="2" t="n">
+        <v>12</v>
+      </c>
+      <c r="F168" s="1" t="s">
+        <v>637</v>
+      </c>
+      <c r="H168" s="5" t="s">
+        <v>638</v>
+      </c>
+      <c r="I168" s="5" t="s">
+        <v>639</v>
+      </c>
+      <c r="J168" s="5" t="s">
+        <v>640</v>
+      </c>
+      <c r="K168" s="5" t="s">
+        <v>641</v>
+      </c>
+    </row>
+    <row r="169" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B169" s="1" t="s">
+        <v>642</v>
+      </c>
+      <c r="C169" s="1" t="s">
+        <v>643</v>
+      </c>
+      <c r="D169" s="2" t="n">
+        <v>32</v>
+      </c>
+      <c r="E169" s="1"/>
+      <c r="F169" s="1" t="s">
+        <v>644</v>
+      </c>
+      <c r="H169" s="1" t="s">
+        <v>645</v>
+      </c>
+      <c r="I169" s="1" t="s">
+        <v>646</v>
+      </c>
+    </row>
+    <row r="170" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A170" s="1" t="n">
+        <v>91</v>
+      </c>
+      <c r="B170" s="1" t="s">
+        <v>647</v>
+      </c>
+      <c r="C170" s="1" t="s">
+        <v>648</v>
+      </c>
+      <c r="D170" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="F170" s="1" t="s">
+        <v>649</v>
+      </c>
+      <c r="H170" s="7" t="s">
+        <v>650</v>
+      </c>
+      <c r="I170" s="7" t="s">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="171" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A171" s="1" t="n">
+        <v>87</v>
+      </c>
+      <c r="B171" s="1" t="s">
+        <v>652</v>
+      </c>
+      <c r="C171" s="1" t="s">
+        <v>653</v>
+      </c>
+      <c r="D171" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="F171" s="1" t="s">
+        <v>654</v>
+      </c>
+      <c r="H171" s="5" t="s">
+        <v>655</v>
+      </c>
+      <c r="I171" s="5" t="s">
+        <v>656</v>
+      </c>
+    </row>
+    <row r="172" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A172" s="3"/>
+      <c r="B172" s="3"/>
+      <c r="C172" s="3"/>
+      <c r="D172" s="4"/>
+      <c r="E172" s="4"/>
+      <c r="F172" s="3"/>
+      <c r="G172" s="3"/>
+      <c r="H172" s="3"/>
+      <c r="I172" s="3"/>
+      <c r="J172" s="3"/>
+      <c r="K172" s="3"/>
+    </row>
+    <row r="173" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A173" s="1" t="n">
+        <v>27</v>
+      </c>
+      <c r="B173" s="1" t="s">
+        <v>657</v>
+      </c>
+      <c r="C173" s="1" t="s">
+        <v>658</v>
+      </c>
+      <c r="D173" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="F167" s="1" t="s">
-        <v>633</v>
-      </c>
-      <c r="H167" s="5" t="s">
-        <v>634</v>
-      </c>
-      <c r="I167" s="5" t="s">
-        <v>635</v>
-      </c>
-    </row>
-    <row r="168" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D168" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="F168" s="1" t="s">
-        <v>636</v>
-      </c>
-      <c r="H168" s="5" t="s">
-        <v>637</v>
-      </c>
-      <c r="I168" s="5" t="s">
-        <v>638</v>
-      </c>
-    </row>
-    <row r="169" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A169" s="1" t="n">
-        <v>37</v>
-      </c>
-      <c r="B169" s="1" t="s">
-        <v>639</v>
-      </c>
-      <c r="C169" s="1" t="s">
-        <v>640</v>
-      </c>
-      <c r="D169" s="2" t="n">
-        <v>12</v>
-      </c>
-      <c r="F169" s="1" t="s">
-        <v>641</v>
-      </c>
-      <c r="H169" s="5" t="s">
-        <v>642</v>
-      </c>
-      <c r="I169" s="5" t="s">
-        <v>643</v>
-      </c>
-      <c r="J169" s="5" t="s">
-        <v>644</v>
-      </c>
-      <c r="K169" s="5" t="s">
-        <v>645</v>
-      </c>
-    </row>
-    <row r="170" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B170" s="1" t="s">
-        <v>646</v>
-      </c>
-      <c r="C170" s="1" t="s">
-        <v>647</v>
-      </c>
-      <c r="D170" s="2" t="n">
-        <v>32</v>
-      </c>
-      <c r="E170" s="1"/>
-      <c r="F170" s="1" t="s">
-        <v>648</v>
-      </c>
-      <c r="H170" s="1" t="s">
-        <v>649</v>
-      </c>
-      <c r="I170" s="1" t="s">
-        <v>650</v>
-      </c>
-    </row>
-    <row r="171" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A171" s="1" t="n">
-        <v>91</v>
-      </c>
-      <c r="B171" s="1" t="s">
-        <v>651</v>
-      </c>
-      <c r="C171" s="1" t="s">
-        <v>652</v>
-      </c>
-      <c r="D171" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="F171" s="1" t="s">
-        <v>653</v>
-      </c>
-      <c r="H171" s="7" t="s">
-        <v>654</v>
-      </c>
-      <c r="I171" s="7" t="s">
-        <v>655</v>
-      </c>
-    </row>
-    <row r="172" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A172" s="1" t="n">
-        <v>87</v>
-      </c>
-      <c r="B172" s="1" t="s">
-        <v>656</v>
-      </c>
-      <c r="C172" s="1" t="s">
-        <v>657</v>
-      </c>
-      <c r="D172" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="F172" s="1" t="s">
-        <v>658</v>
-      </c>
-      <c r="H172" s="5" t="s">
+      <c r="F173" s="1" t="s">
         <v>659</v>
       </c>
-      <c r="I172" s="5" t="s">
+      <c r="H173" s="7" t="s">
         <v>660</v>
       </c>
-    </row>
-    <row r="173" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A173" s="3"/>
-      <c r="B173" s="3"/>
-      <c r="C173" s="3"/>
-      <c r="D173" s="4"/>
-      <c r="E173" s="4"/>
-      <c r="F173" s="3"/>
-      <c r="G173" s="3"/>
-      <c r="H173" s="3"/>
-      <c r="I173" s="3"/>
-      <c r="J173" s="3"/>
-      <c r="K173" s="3"/>
-    </row>
-    <row r="174" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I173" s="7" t="s">
+        <v>661</v>
+      </c>
+    </row>
+    <row r="174" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A174" s="1" t="n">
-        <v>27</v>
+        <v>126</v>
       </c>
       <c r="B174" s="1" t="s">
-        <v>661</v>
+        <v>662</v>
       </c>
       <c r="C174" s="1" t="s">
-        <v>662</v>
+        <v>663</v>
       </c>
       <c r="D174" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="F174" s="1" t="s">
+        <v>664</v>
+      </c>
+      <c r="H174" s="1" t="s">
+        <v>665</v>
+      </c>
+      <c r="I174" s="1" t="s">
+        <v>666</v>
+      </c>
+      <c r="J174" s="1" t="s">
+        <v>667</v>
+      </c>
+      <c r="K174" s="1" t="s">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="175" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A175" s="3"/>
+      <c r="B175" s="3"/>
+      <c r="C175" s="3"/>
+      <c r="D175" s="4"/>
+      <c r="E175" s="4"/>
+      <c r="F175" s="3"/>
+      <c r="G175" s="3"/>
+      <c r="H175" s="3"/>
+      <c r="I175" s="3"/>
+      <c r="J175" s="3"/>
+      <c r="K175" s="3"/>
+    </row>
+    <row r="176" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A176" s="1" t="n">
+        <v>48</v>
+      </c>
+      <c r="B176" s="1" t="s">
+        <v>669</v>
+      </c>
+      <c r="C176" s="1" t="s">
+        <v>670</v>
+      </c>
+      <c r="D176" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="F176" s="1" t="s">
+        <v>671</v>
+      </c>
+      <c r="H176" s="5" t="s">
+        <v>672</v>
+      </c>
+      <c r="I176" s="8" t="s">
+        <v>673</v>
+      </c>
+    </row>
+    <row r="177" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A177" s="1" t="n">
+        <v>69</v>
+      </c>
+      <c r="B177" s="1" t="s">
+        <v>674</v>
+      </c>
+      <c r="C177" s="1" t="s">
+        <v>675</v>
+      </c>
+      <c r="D177" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="F177" s="1" t="s">
+        <v>676</v>
+      </c>
+      <c r="H177" s="7" t="s">
+        <v>677</v>
+      </c>
+      <c r="I177" s="7" t="s">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="178" s="13" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A178" s="1" t="n">
+        <v>79</v>
+      </c>
+      <c r="B178" s="1" t="s">
+        <v>679</v>
+      </c>
+      <c r="C178" s="1" t="s">
+        <v>680</v>
+      </c>
+      <c r="D178" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="E178" s="2"/>
+      <c r="F178" s="1" t="s">
+        <v>681</v>
+      </c>
+      <c r="G178" s="1"/>
+      <c r="H178" s="7" t="s">
+        <v>682</v>
+      </c>
+      <c r="I178" s="7" t="s">
+        <v>683</v>
+      </c>
+      <c r="J178" s="1"/>
+      <c r="K178" s="1"/>
+      <c r="L178" s="1"/>
+    </row>
+    <row r="179" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A179" s="1" t="n">
+        <v>136</v>
+      </c>
+      <c r="B179" s="1" t="s">
+        <v>684</v>
+      </c>
+      <c r="C179" s="1" t="s">
+        <v>685</v>
+      </c>
+      <c r="D179" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="F179" s="1" t="s">
+        <v>686</v>
+      </c>
+      <c r="H179" s="5" t="s">
+        <v>687</v>
+      </c>
+      <c r="I179" s="5" t="s">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="180" s="13" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A180" s="13" t="n">
+        <v>149</v>
+      </c>
+      <c r="B180" s="13" t="s">
+        <v>689</v>
+      </c>
+      <c r="C180" s="13" t="s">
+        <v>670</v>
+      </c>
+      <c r="D180" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E180" s="14" t="n">
+        <v>1</v>
+      </c>
+      <c r="F180" s="13" t="s">
+        <v>690</v>
+      </c>
+      <c r="H180" s="15" t="s">
+        <v>691</v>
+      </c>
+      <c r="I180" s="15" t="s">
+        <v>692</v>
+      </c>
+      <c r="J180" s="15" t="s">
+        <v>693</v>
+      </c>
+      <c r="K180" s="15" t="s">
+        <v>694</v>
+      </c>
+      <c r="L180" s="1"/>
+    </row>
+    <row r="181" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A181" s="3"/>
+      <c r="B181" s="3"/>
+      <c r="C181" s="3"/>
+      <c r="D181" s="4"/>
+      <c r="E181" s="4"/>
+      <c r="F181" s="3"/>
+      <c r="G181" s="3"/>
+      <c r="H181" s="3"/>
+      <c r="I181" s="3"/>
+      <c r="J181" s="3"/>
+      <c r="K181" s="3"/>
+    </row>
+    <row r="182" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A182" s="13" t="n">
+        <v>89</v>
+      </c>
+      <c r="B182" s="13" t="s">
+        <v>695</v>
+      </c>
+      <c r="C182" s="13" t="s">
+        <v>696</v>
+      </c>
+      <c r="D182" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E182" s="14" t="n">
+        <v>1</v>
+      </c>
+      <c r="F182" s="13" t="s">
+        <v>697</v>
+      </c>
+      <c r="G182" s="13"/>
+      <c r="H182" s="13" t="s">
+        <v>698</v>
+      </c>
+      <c r="I182" s="13" t="s">
+        <v>699</v>
+      </c>
+      <c r="J182" s="13"/>
+      <c r="K182" s="13"/>
+    </row>
+    <row r="183" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D183" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="F183" s="5" t="s">
+        <v>700</v>
+      </c>
+      <c r="H183" s="5" t="s">
+        <v>701</v>
+      </c>
+      <c r="I183" s="5" t="s">
+        <v>702</v>
+      </c>
+    </row>
+    <row r="184" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A184" s="1" t="n">
+        <v>122</v>
+      </c>
+      <c r="B184" s="1" t="s">
+        <v>703</v>
+      </c>
+      <c r="C184" s="1" t="s">
+        <v>704</v>
+      </c>
+      <c r="D184" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="F184" s="1" t="s">
+        <v>705</v>
+      </c>
+      <c r="H184" s="5" t="s">
+        <v>706</v>
+      </c>
+      <c r="I184" s="5" t="s">
+        <v>707</v>
+      </c>
+    </row>
+    <row r="185" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D185" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="F174" s="1" t="s">
-        <v>663</v>
-      </c>
-      <c r="H174" s="7" t="s">
-        <v>664</v>
-      </c>
-      <c r="I174" s="7" t="s">
-        <v>665</v>
-      </c>
-    </row>
-    <row r="175" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A175" s="1" t="n">
-        <v>126</v>
-      </c>
-      <c r="B175" s="1" t="s">
-        <v>666</v>
-      </c>
-      <c r="C175" s="1" t="s">
-        <v>667</v>
-      </c>
-      <c r="D175" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="F175" s="1" t="s">
-        <v>668</v>
-      </c>
-      <c r="H175" s="1" t="s">
-        <v>669</v>
-      </c>
-      <c r="I175" s="1" t="s">
-        <v>670</v>
-      </c>
-      <c r="J175" s="1" t="s">
-        <v>671</v>
-      </c>
-      <c r="K175" s="1" t="s">
-        <v>672</v>
-      </c>
-    </row>
-    <row r="176" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A176" s="3"/>
-      <c r="B176" s="3"/>
-      <c r="C176" s="3"/>
-      <c r="D176" s="4"/>
-      <c r="E176" s="4"/>
-      <c r="F176" s="3"/>
-      <c r="G176" s="3"/>
-      <c r="H176" s="3"/>
-      <c r="I176" s="3"/>
-      <c r="J176" s="3"/>
-      <c r="K176" s="3"/>
-    </row>
-    <row r="177" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A177" s="1" t="n">
-        <v>48</v>
-      </c>
-      <c r="B177" s="1" t="s">
-        <v>673</v>
-      </c>
-      <c r="C177" s="1" t="s">
-        <v>674</v>
-      </c>
-      <c r="D177" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="F177" s="1" t="s">
-        <v>675</v>
-      </c>
-      <c r="H177" s="5" t="s">
-        <v>676</v>
-      </c>
-      <c r="I177" s="8" t="s">
-        <v>677</v>
-      </c>
-    </row>
-    <row r="178" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A178" s="1" t="n">
-        <v>69</v>
-      </c>
-      <c r="B178" s="1" t="s">
-        <v>678</v>
-      </c>
-      <c r="C178" s="1" t="s">
-        <v>679</v>
-      </c>
-      <c r="D178" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="F178" s="1" t="s">
-        <v>680</v>
-      </c>
-      <c r="H178" s="7" t="s">
-        <v>681</v>
-      </c>
-      <c r="I178" s="7" t="s">
-        <v>682</v>
-      </c>
-    </row>
-    <row r="179" s="13" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A179" s="1" t="n">
-        <v>79</v>
-      </c>
-      <c r="B179" s="1" t="s">
-        <v>683</v>
-      </c>
-      <c r="C179" s="1" t="s">
-        <v>684</v>
-      </c>
-      <c r="D179" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="E179" s="2"/>
-      <c r="F179" s="1" t="s">
-        <v>685</v>
-      </c>
-      <c r="G179" s="1"/>
-      <c r="H179" s="7" t="s">
-        <v>686</v>
-      </c>
-      <c r="I179" s="7" t="s">
-        <v>687</v>
-      </c>
-      <c r="J179" s="1"/>
-      <c r="K179" s="1"/>
-      <c r="L179" s="1"/>
-    </row>
-    <row r="180" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A180" s="1" t="n">
-        <v>136</v>
-      </c>
-      <c r="B180" s="1" t="s">
-        <v>688</v>
-      </c>
-      <c r="C180" s="1" t="s">
-        <v>689</v>
-      </c>
-      <c r="D180" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="F180" s="1" t="s">
-        <v>690</v>
-      </c>
-      <c r="H180" s="5" t="s">
-        <v>691</v>
-      </c>
-      <c r="I180" s="5" t="s">
-        <v>692</v>
-      </c>
-    </row>
-    <row r="181" s="13" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A181" s="13" t="n">
-        <v>149</v>
-      </c>
-      <c r="B181" s="13" t="s">
-        <v>693</v>
-      </c>
-      <c r="C181" s="13" t="s">
-        <v>674</v>
-      </c>
-      <c r="D181" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E181" s="14" t="n">
-        <v>1</v>
-      </c>
-      <c r="F181" s="13" t="s">
-        <v>694</v>
-      </c>
-      <c r="H181" s="15" t="s">
-        <v>695</v>
-      </c>
-      <c r="I181" s="15" t="s">
-        <v>696</v>
-      </c>
-      <c r="J181" s="15" t="s">
-        <v>697</v>
-      </c>
-      <c r="K181" s="15" t="s">
-        <v>698</v>
-      </c>
-      <c r="L181" s="1"/>
-    </row>
-    <row r="182" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A182" s="3"/>
-      <c r="B182" s="3"/>
-      <c r="C182" s="3"/>
-      <c r="D182" s="4"/>
-      <c r="E182" s="4"/>
-      <c r="F182" s="3"/>
-      <c r="G182" s="3"/>
-      <c r="H182" s="3"/>
-      <c r="I182" s="3"/>
-      <c r="J182" s="3"/>
-      <c r="K182" s="3"/>
-    </row>
-    <row r="183" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A183" s="13" t="n">
-        <v>89</v>
-      </c>
-      <c r="B183" s="13" t="s">
-        <v>699</v>
-      </c>
-      <c r="C183" s="13" t="s">
+      <c r="F185" s="5" t="s">
         <v>700</v>
       </c>
-      <c r="D183" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E183" s="14" t="n">
-        <v>1</v>
-      </c>
-      <c r="F183" s="13" t="s">
-        <v>701</v>
-      </c>
-      <c r="G183" s="13"/>
-      <c r="H183" s="13" t="s">
-        <v>702</v>
-      </c>
-      <c r="I183" s="13" t="s">
-        <v>703</v>
-      </c>
-      <c r="J183" s="13"/>
-      <c r="K183" s="13"/>
-    </row>
-    <row r="184" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D184" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="F184" s="5" t="s">
-        <v>704</v>
-      </c>
-      <c r="H184" s="5" t="s">
-        <v>705</v>
-      </c>
-      <c r="I184" s="5" t="s">
-        <v>706</v>
-      </c>
-    </row>
-    <row r="185" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A185" s="1" t="n">
-        <v>122</v>
-      </c>
-      <c r="B185" s="1" t="s">
-        <v>707</v>
-      </c>
-      <c r="C185" s="1" t="s">
+      <c r="H185" s="1" t="s">
         <v>708</v>
       </c>
-      <c r="D185" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="F185" s="1" t="s">
+      <c r="I185" s="1" t="s">
         <v>709</v>
       </c>
-      <c r="H185" s="5" t="s">
+      <c r="J185" s="7" t="s">
         <v>710</v>
       </c>
-      <c r="I185" s="5" t="s">
+      <c r="K185" s="7" t="s">
         <v>711</v>
       </c>
     </row>
     <row r="186" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A186" s="1" t="n">
+        <v>154</v>
+      </c>
+      <c r="B186" s="1" t="s">
+        <v>712</v>
+      </c>
+      <c r="C186" s="1" t="s">
+        <v>713</v>
+      </c>
       <c r="D186" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="F186" s="5" t="s">
-        <v>704</v>
-      </c>
-      <c r="H186" s="1" t="s">
-        <v>712</v>
-      </c>
-      <c r="I186" s="1" t="s">
-        <v>713</v>
-      </c>
-      <c r="J186" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="F186" s="1" t="s">
         <v>714</v>
       </c>
-      <c r="K186" s="7" t="s">
+      <c r="H186" s="7" t="s">
         <v>715</v>
+      </c>
+      <c r="I186" s="7" t="s">
+        <v>716</v>
       </c>
     </row>
     <row r="187" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A187" s="1" t="n">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B187" s="1" t="s">
-        <v>716</v>
+        <v>717</v>
       </c>
       <c r="C187" s="1" t="s">
-        <v>717</v>
+        <v>718</v>
       </c>
       <c r="D187" s="2" t="n">
         <v>1</v>
       </c>
       <c r="F187" s="1" t="s">
-        <v>718</v>
+        <v>182</v>
       </c>
       <c r="H187" s="7" t="s">
         <v>719</v>
@@ -6866,106 +6854,83 @@
       </c>
     </row>
     <row r="188" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A188" s="1" t="n">
-        <v>155</v>
-      </c>
-      <c r="B188" s="1" t="s">
+      <c r="D188" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="F188" s="5" t="s">
+        <v>700</v>
+      </c>
+      <c r="H188" s="7" t="s">
         <v>721</v>
       </c>
-      <c r="C188" s="1" t="s">
+      <c r="I188" s="7" t="s">
         <v>722</v>
       </c>
-      <c r="D188" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="F188" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="H188" s="7" t="s">
+    </row>
+    <row r="189" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A189" s="3"/>
+      <c r="B189" s="3"/>
+      <c r="C189" s="3"/>
+      <c r="D189" s="4"/>
+      <c r="E189" s="4"/>
+      <c r="F189" s="3"/>
+      <c r="G189" s="3"/>
+      <c r="H189" s="3"/>
+      <c r="I189" s="3"/>
+      <c r="J189" s="3"/>
+      <c r="K189" s="3"/>
+    </row>
+    <row r="191" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B191" s="1" t="s">
         <v>723</v>
       </c>
-      <c r="I188" s="7" t="s">
+      <c r="D191" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="H191" s="1" t="s">
         <v>724</v>
       </c>
-    </row>
-    <row r="189" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D189" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="F189" s="5" t="s">
-        <v>704</v>
-      </c>
-      <c r="H189" s="7" t="s">
-        <v>725</v>
-      </c>
-      <c r="I189" s="7" t="s">
-        <v>726</v>
-      </c>
-    </row>
-    <row r="190" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A190" s="3"/>
-      <c r="B190" s="3"/>
-      <c r="C190" s="3"/>
-      <c r="D190" s="4"/>
-      <c r="E190" s="4"/>
-      <c r="F190" s="3"/>
-      <c r="G190" s="3"/>
-      <c r="H190" s="3"/>
-      <c r="I190" s="3"/>
-      <c r="J190" s="3"/>
-      <c r="K190" s="3"/>
+      <c r="I191" s="16" t="n">
+        <v>830207670409</v>
+      </c>
     </row>
     <row r="192" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B192" s="1" t="s">
+        <v>725</v>
+      </c>
+      <c r="D192" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="H192" s="1" t="s">
+        <v>726</v>
+      </c>
+      <c r="I192" s="1" t="s">
         <v>727</v>
-      </c>
-      <c r="D192" s="2" t="n">
-        <v>3</v>
-      </c>
-      <c r="H192" s="1" t="s">
-        <v>728</v>
-      </c>
-      <c r="I192" s="16" t="n">
-        <v>830207670409</v>
       </c>
     </row>
     <row r="193" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B193" s="1" t="s">
-        <v>729</v>
+        <v>725</v>
       </c>
       <c r="D193" s="2" t="n">
         <v>2</v>
       </c>
       <c r="H193" s="1" t="s">
+        <v>728</v>
+      </c>
+      <c r="I193" s="1" t="s">
+        <v>729</v>
+      </c>
+    </row>
+    <row r="195" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B195" s="1" t="s">
         <v>730</v>
       </c>
-      <c r="I193" s="1" t="s">
+      <c r="H195" s="1" t="s">
         <v>731</v>
       </c>
-    </row>
-    <row r="194" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B194" s="1" t="s">
-        <v>729</v>
-      </c>
-      <c r="D194" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="H194" s="1" t="s">
+      <c r="I195" s="1" t="s">
         <v>732</v>
-      </c>
-      <c r="I194" s="1" t="s">
-        <v>733</v>
-      </c>
-    </row>
-    <row r="196" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B196" s="1" t="s">
-        <v>734</v>
-      </c>
-      <c r="H196" s="1" t="s">
-        <v>735</v>
-      </c>
-      <c r="I196" s="1" t="s">
-        <v>736</v>
       </c>
     </row>
   </sheetData>

</xml_diff>